<commit_message>
Running test specifications, adding comments, and defining function for inflation target estimate
</commit_message>
<xml_diff>
--- a/Complied Data.xlsx
+++ b/Complied Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Honours-Project1\R Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\R-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218CD245-268B-457A-A57A-AA789546D825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2503AE-F757-4D8D-ACE2-24FBBA43AAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="105">
   <si>
     <t>Dates</t>
   </si>
@@ -392,14 +392,20 @@
   <si>
     <t>ADPYEG</t>
   </si>
+  <si>
+    <t>Glen Stevens</t>
+  </si>
+  <si>
+    <t>Phillip Lowe</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0;\-0.0;0.0;@"/>
-    <numFmt numFmtId="166" formatCode="0.00;\-0.00;0.00;@"/>
+    <numFmt numFmtId="164" formatCode="0.0;\-0.0;0.0;@"/>
+    <numFmt numFmtId="165" formatCode="0.00;\-0.00;0.00;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -479,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -507,8 +513,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,12 +818,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BT161"/>
+  <dimension ref="A1:BV161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AT1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="BX15" sqref="BX15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -824,7 +831,7 @@
     <col min="1" max="1" width="18.26953125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" ht="71.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:74" ht="71.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1041,8 +1048,14 @@
       <c r="BT1" s="7" t="s">
         <v>102</v>
       </c>
+      <c r="BU1" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="BV1" s="13" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="2" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>38993</v>
       </c>
@@ -1247,8 +1260,14 @@
       <c r="BT2" s="12">
         <v>4.5393858477970513E-2</v>
       </c>
+      <c r="BU2">
+        <v>1</v>
+      </c>
+      <c r="BV2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>39028</v>
       </c>
@@ -1453,8 +1472,14 @@
       <c r="BT3" s="12">
         <v>4.5393858477970513E-2</v>
       </c>
+      <c r="BU3">
+        <v>1</v>
+      </c>
+      <c r="BV3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>39056</v>
       </c>
@@ -1659,8 +1684,14 @@
       <c r="BT4" s="12">
         <v>5.5702917771883131E-2</v>
       </c>
+      <c r="BU4">
+        <v>1</v>
+      </c>
+      <c r="BV4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>39119</v>
       </c>
@@ -1865,8 +1896,14 @@
       <c r="BT5" s="12">
         <v>5.5702917771883131E-2</v>
       </c>
+      <c r="BU5">
+        <v>1</v>
+      </c>
+      <c r="BV5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>39147</v>
       </c>
@@ -2071,8 +2108,14 @@
       <c r="BT6" s="12">
         <v>4.5931758530183726E-2</v>
       </c>
+      <c r="BU6">
+        <v>1</v>
+      </c>
+      <c r="BV6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>39175</v>
       </c>
@@ -2277,8 +2320,14 @@
       <c r="BT7" s="12">
         <v>4.5931758530183726E-2</v>
       </c>
+      <c r="BU7">
+        <v>1</v>
+      </c>
+      <c r="BV7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>39203</v>
       </c>
@@ -2483,8 +2532,14 @@
       <c r="BT8" s="12">
         <v>4.5931758530183726E-2</v>
       </c>
+      <c r="BU8">
+        <v>1</v>
+      </c>
+      <c r="BV8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>39238</v>
       </c>
@@ -2689,8 +2744,14 @@
       <c r="BT9" s="12">
         <v>6.7688378033205585E-2</v>
       </c>
+      <c r="BU9">
+        <v>1</v>
+      </c>
+      <c r="BV9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>39266</v>
       </c>
@@ -2895,8 +2956,14 @@
       <c r="BT10" s="12">
         <v>6.7688378033205585E-2</v>
       </c>
+      <c r="BU10">
+        <v>1</v>
+      </c>
+      <c r="BV10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>39301</v>
       </c>
@@ -3101,8 +3168,14 @@
       <c r="BT11" s="12">
         <v>6.7688378033205585E-2</v>
       </c>
+      <c r="BU11">
+        <v>1</v>
+      </c>
+      <c r="BV11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>39329</v>
       </c>
@@ -3307,8 +3380,14 @@
       <c r="BT12" s="12">
         <v>9.8339719029374245E-2</v>
       </c>
+      <c r="BU12">
+        <v>1</v>
+      </c>
+      <c r="BV12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>39357</v>
       </c>
@@ -3513,8 +3592,14 @@
       <c r="BT13" s="12">
         <v>9.8339719029374245E-2</v>
       </c>
+      <c r="BU13">
+        <v>1</v>
+      </c>
+      <c r="BV13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>39392</v>
       </c>
@@ -3719,8 +3804,14 @@
       <c r="BT14" s="12">
         <v>9.8339719029374245E-2</v>
       </c>
+      <c r="BU14">
+        <v>1</v>
+      </c>
+      <c r="BV14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>39420</v>
       </c>
@@ -3925,8 +4016,14 @@
       <c r="BT15" s="12">
         <v>0.10678391959798995</v>
       </c>
+      <c r="BU15">
+        <v>1</v>
+      </c>
+      <c r="BV15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>39483</v>
       </c>
@@ -4131,8 +4228,14 @@
       <c r="BT16" s="12">
         <v>0.10678391959798995</v>
       </c>
+      <c r="BU16">
+        <v>1</v>
+      </c>
+      <c r="BV16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>39511</v>
       </c>
@@ -4337,8 +4440,14 @@
       <c r="BT17" s="12">
         <v>9.9121706398996132E-2</v>
       </c>
+      <c r="BU17">
+        <v>1</v>
+      </c>
+      <c r="BV17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>39539</v>
       </c>
@@ -4543,8 +4652,14 @@
       <c r="BT18" s="12">
         <v>9.9121706398996132E-2</v>
       </c>
+      <c r="BU18">
+        <v>1</v>
+      </c>
+      <c r="BV18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>39574</v>
       </c>
@@ -4758,8 +4873,14 @@
       <c r="BT19" s="12">
         <v>9.9121706398996132E-2</v>
       </c>
+      <c r="BU19">
+        <v>1</v>
+      </c>
+      <c r="BV19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>39602</v>
       </c>
@@ -4973,8 +5094,14 @@
       <c r="BT20" s="12">
         <v>3.9473684210526452E-2</v>
       </c>
+      <c r="BU20">
+        <v>1</v>
+      </c>
+      <c r="BV20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>39630</v>
       </c>
@@ -5188,8 +5315,14 @@
       <c r="BT21" s="12">
         <v>3.9473684210526452E-2</v>
       </c>
+      <c r="BU21">
+        <v>1</v>
+      </c>
+      <c r="BV21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>39665</v>
       </c>
@@ -5403,8 +5536,14 @@
       <c r="BT22" s="12">
         <v>3.9473684210526452E-2</v>
       </c>
+      <c r="BU22">
+        <v>1</v>
+      </c>
+      <c r="BV22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>39693</v>
       </c>
@@ -5618,8 +5757,14 @@
       <c r="BT23" s="12">
         <v>-2.3255813953488701E-3</v>
       </c>
+      <c r="BU23">
+        <v>1</v>
+      </c>
+      <c r="BV23">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>39728</v>
       </c>
@@ -5833,8 +5978,14 @@
       <c r="BT24" s="12">
         <v>-2.3255813953488701E-3</v>
       </c>
+      <c r="BU24">
+        <v>1</v>
+      </c>
+      <c r="BV24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>39756</v>
       </c>
@@ -6051,8 +6202,14 @@
       <c r="BT25" s="12">
         <v>-2.3255813953488701E-3</v>
       </c>
+      <c r="BU25">
+        <v>1</v>
+      </c>
+      <c r="BV25">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>39784</v>
       </c>
@@ -6269,8 +6426,14 @@
       <c r="BT26" s="12">
         <v>-3.5187287173666225E-2</v>
       </c>
+      <c r="BU26">
+        <v>1</v>
+      </c>
+      <c r="BV26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>39847</v>
       </c>
@@ -6487,8 +6650,14 @@
       <c r="BT27" s="12">
         <v>-3.5187287173666225E-2</v>
       </c>
+      <c r="BU27">
+        <v>1</v>
+      </c>
+      <c r="BV27">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>39875</v>
       </c>
@@ -6705,8 +6874,14 @@
       <c r="BT28" s="12">
         <v>-1.4840182648401794E-2</v>
       </c>
+      <c r="BU28">
+        <v>1</v>
+      </c>
+      <c r="BV28">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>39910</v>
       </c>
@@ -6923,8 +7098,14 @@
       <c r="BT29" s="12">
         <v>-1.4840182648401794E-2</v>
       </c>
+      <c r="BU29">
+        <v>1</v>
+      </c>
+      <c r="BV29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>39938</v>
       </c>
@@ -7141,8 +7322,14 @@
       <c r="BT30" s="12">
         <v>-1.4840182648401794E-2</v>
       </c>
+      <c r="BU30">
+        <v>1</v>
+      </c>
+      <c r="BV30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>39966</v>
       </c>
@@ -7359,8 +7546,14 @@
       <c r="BT31" s="12">
         <v>2.8768699654775604E-2</v>
       </c>
+      <c r="BU31">
+        <v>1</v>
+      </c>
+      <c r="BV31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>40001</v>
       </c>
@@ -7577,8 +7770,14 @@
       <c r="BT32" s="12">
         <v>2.8768699654775604E-2</v>
       </c>
+      <c r="BU32">
+        <v>1</v>
+      </c>
+      <c r="BV32">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>40029</v>
       </c>
@@ -7795,8 +7994,14 @@
       <c r="BT33" s="12">
         <v>2.8768699654775604E-2</v>
       </c>
+      <c r="BU33">
+        <v>1</v>
+      </c>
+      <c r="BV33">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>40057</v>
       </c>
@@ -8013,8 +8218,14 @@
       <c r="BT34" s="12">
         <v>8.0419580419580486E-2</v>
       </c>
+      <c r="BU34">
+        <v>1</v>
+      </c>
+      <c r="BV34">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>40092</v>
       </c>
@@ -8231,8 +8442,14 @@
       <c r="BT35" s="12">
         <v>8.0419580419580486E-2</v>
       </c>
+      <c r="BU35">
+        <v>1</v>
+      </c>
+      <c r="BV35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>40120</v>
       </c>
@@ -8449,8 +8666,14 @@
       <c r="BT36" s="12">
         <v>8.0419580419580486E-2</v>
       </c>
+      <c r="BU36">
+        <v>1</v>
+      </c>
+      <c r="BV36">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>40148</v>
       </c>
@@ -8667,8 +8890,14 @@
       <c r="BT37" s="12">
         <v>0.15058823529411761</v>
       </c>
+      <c r="BU37">
+        <v>1</v>
+      </c>
+      <c r="BV37">
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>40211</v>
       </c>
@@ -8885,8 +9114,14 @@
       <c r="BT38" s="12">
         <v>0.15058823529411761</v>
       </c>
+      <c r="BU38">
+        <v>1</v>
+      </c>
+      <c r="BV38">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>40239</v>
       </c>
@@ -9103,8 +9338,14 @@
       <c r="BT39" s="12">
         <v>0.15990730011587484</v>
       </c>
+      <c r="BU39">
+        <v>1</v>
+      </c>
+      <c r="BV39">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>40274</v>
       </c>
@@ -9321,8 +9562,14 @@
       <c r="BT40" s="12">
         <v>0.15990730011587484</v>
       </c>
+      <c r="BU40">
+        <v>1</v>
+      </c>
+      <c r="BV40">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>40302</v>
       </c>
@@ -9539,8 +9786,14 @@
       <c r="BT41" s="12">
         <v>0.15990730011587484</v>
       </c>
+      <c r="BU41">
+        <v>1</v>
+      </c>
+      <c r="BV41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>40330</v>
       </c>
@@ -9757,8 +10010,14 @@
       <c r="BT42" s="12">
         <v>0.1420581655480983</v>
       </c>
+      <c r="BU42">
+        <v>1</v>
+      </c>
+      <c r="BV42">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>40365</v>
       </c>
@@ -9975,8 +10234,14 @@
       <c r="BT43" s="12">
         <v>0.1420581655480983</v>
       </c>
+      <c r="BU43">
+        <v>1</v>
+      </c>
+      <c r="BV43">
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>40393</v>
       </c>
@@ -10193,8 +10458,14 @@
       <c r="BT44" s="12">
         <v>0.1420581655480983</v>
       </c>
+      <c r="BU44">
+        <v>1</v>
+      </c>
+      <c r="BV44">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>40428</v>
       </c>
@@ -10411,8 +10682,14 @@
       <c r="BT45" s="12">
         <v>8.8457389428263242E-2</v>
       </c>
+      <c r="BU45">
+        <v>1</v>
+      </c>
+      <c r="BV45">
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>40456</v>
       </c>
@@ -10629,8 +10906,14 @@
       <c r="BT46" s="12">
         <v>8.8457389428263242E-2</v>
       </c>
+      <c r="BU46">
+        <v>1</v>
+      </c>
+      <c r="BV46">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>40484</v>
       </c>
@@ -10847,8 +11130,14 @@
       <c r="BT47" s="12">
         <v>8.8457389428263242E-2</v>
       </c>
+      <c r="BU47">
+        <v>1</v>
+      </c>
+      <c r="BV47">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>40519</v>
       </c>
@@ -11065,8 +11354,14 @@
       <c r="BT48" s="12">
         <v>3.9877300613496994E-2</v>
       </c>
+      <c r="BU48">
+        <v>1</v>
+      </c>
+      <c r="BV48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>40575</v>
       </c>
@@ -11283,8 +11578,14 @@
       <c r="BT49" s="12">
         <v>3.9877300613496994E-2</v>
       </c>
+      <c r="BU49">
+        <v>1</v>
+      </c>
+      <c r="BV49">
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>40603</v>
       </c>
@@ -11501,8 +11802,14 @@
       <c r="BT50" s="12">
         <v>1.1988011988012017E-2</v>
       </c>
+      <c r="BU50">
+        <v>1</v>
+      </c>
+      <c r="BV50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>40638</v>
       </c>
@@ -11719,8 +12026,14 @@
       <c r="BT51" s="12">
         <v>1.1988011988012017E-2</v>
       </c>
+      <c r="BU51">
+        <v>1</v>
+      </c>
+      <c r="BV51">
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>40666</v>
       </c>
@@ -11937,8 +12250,14 @@
       <c r="BT52" s="12">
         <v>1.1988011988012017E-2</v>
       </c>
+      <c r="BU52">
+        <v>1</v>
+      </c>
+      <c r="BV52">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>40701</v>
       </c>
@@ -12155,8 +12474,14 @@
       <c r="BT53" s="12">
         <v>-6.8560235063661965E-3</v>
       </c>
+      <c r="BU53">
+        <v>1</v>
+      </c>
+      <c r="BV53">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>40729</v>
       </c>
@@ -12373,8 +12698,14 @@
       <c r="BT54" s="12">
         <v>-6.8560235063661965E-3</v>
       </c>
+      <c r="BU54">
+        <v>1</v>
+      </c>
+      <c r="BV54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>40757</v>
       </c>
@@ -12591,8 +12922,14 @@
       <c r="BT55" s="12">
         <v>-6.8560235063661965E-3</v>
       </c>
+      <c r="BU55">
+        <v>1</v>
+      </c>
+      <c r="BV55">
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>40792</v>
       </c>
@@ -12809,8 +13146,14 @@
       <c r="BT56" s="12">
         <v>-8.9197224975223546E-3</v>
       </c>
+      <c r="BU56">
+        <v>1</v>
+      </c>
+      <c r="BV56">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>40820</v>
       </c>
@@ -13027,8 +13370,14 @@
       <c r="BT57" s="12">
         <v>-8.9197224975223546E-3</v>
       </c>
+      <c r="BU57">
+        <v>1</v>
+      </c>
+      <c r="BV57">
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>40848</v>
       </c>
@@ -13245,8 +13594,14 @@
       <c r="BT58" s="12">
         <v>-8.9197224975223546E-3</v>
       </c>
+      <c r="BU58">
+        <v>1</v>
+      </c>
+      <c r="BV58">
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>40883</v>
       </c>
@@ -13463,8 +13818,14 @@
       <c r="BT59" s="12">
         <v>-2.9498525073746312E-2</v>
       </c>
+      <c r="BU59">
+        <v>1</v>
+      </c>
+      <c r="BV59">
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>40946</v>
       </c>
@@ -13681,8 +14042,14 @@
       <c r="BT60" s="12">
         <v>-2.9498525073746312E-2</v>
       </c>
+      <c r="BU60">
+        <v>1</v>
+      </c>
+      <c r="BV60">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>40974</v>
       </c>
@@ -13899,8 +14266,14 @@
       <c r="BT61" s="12">
         <v>-4.9358341559723592E-3</v>
       </c>
+      <c r="BU61">
+        <v>1</v>
+      </c>
+      <c r="BV61">
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>41002</v>
       </c>
@@ -14117,8 +14490,14 @@
       <c r="BT62" s="12">
         <v>-4.9358341559723592E-3</v>
       </c>
+      <c r="BU62">
+        <v>1</v>
+      </c>
+      <c r="BV62">
+        <v>0</v>
+      </c>
     </row>
-    <row r="63" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>41030</v>
       </c>
@@ -14335,8 +14714,14 @@
       <c r="BT63" s="12">
         <v>-4.9358341559723592E-3</v>
       </c>
+      <c r="BU63">
+        <v>1</v>
+      </c>
+      <c r="BV63">
+        <v>0</v>
+      </c>
     </row>
-    <row r="64" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>41065</v>
       </c>
@@ -14553,8 +14938,14 @@
       <c r="BT64" s="12">
         <v>-8.8757396449704699E-3</v>
       </c>
+      <c r="BU64">
+        <v>1</v>
+      </c>
+      <c r="BV64">
+        <v>0</v>
+      </c>
     </row>
-    <row r="65" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>41093</v>
       </c>
@@ -14771,8 +15162,14 @@
       <c r="BT65" s="12">
         <v>-8.8757396449704699E-3</v>
       </c>
+      <c r="BU65">
+        <v>1</v>
+      </c>
+      <c r="BV65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>41128</v>
       </c>
@@ -14989,8 +15386,14 @@
       <c r="BT66" s="12">
         <v>-8.8757396449704699E-3</v>
       </c>
+      <c r="BU66">
+        <v>1</v>
+      </c>
+      <c r="BV66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>41156</v>
       </c>
@@ -15207,8 +15610,14 @@
       <c r="BT67" s="12">
         <v>5.0000000000000001E-3</v>
       </c>
+      <c r="BU67">
+        <v>1</v>
+      </c>
+      <c r="BV67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>41184</v>
       </c>
@@ -15425,8 +15834,14 @@
       <c r="BT68" s="12">
         <v>5.0000000000000001E-3</v>
       </c>
+      <c r="BU68">
+        <v>1</v>
+      </c>
+      <c r="BV68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>41219</v>
       </c>
@@ -15643,8 +16058,14 @@
       <c r="BT69" s="12">
         <v>5.0000000000000001E-3</v>
       </c>
+      <c r="BU69">
+        <v>1</v>
+      </c>
+      <c r="BV69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>41247</v>
       </c>
@@ -15861,8 +16282,14 @@
       <c r="BT70" s="12">
         <v>4.0526849037487336E-2</v>
       </c>
+      <c r="BU70">
+        <v>1</v>
+      </c>
+      <c r="BV70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>41310</v>
       </c>
@@ -16079,8 +16506,14 @@
       <c r="BT71" s="12">
         <v>4.0526849037487336E-2</v>
       </c>
+      <c r="BU71">
+        <v>1</v>
+      </c>
+      <c r="BV71">
+        <v>0</v>
+      </c>
     </row>
-    <row r="72" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>41338</v>
       </c>
@@ -16297,8 +16730,14 @@
       <c r="BT72" s="12">
         <v>2.5793650793650879E-2</v>
       </c>
+      <c r="BU72">
+        <v>1</v>
+      </c>
+      <c r="BV72">
+        <v>0</v>
+      </c>
     </row>
-    <row r="73" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>41366</v>
       </c>
@@ -16515,8 +16954,14 @@
       <c r="BT73" s="12">
         <v>2.5793650793650879E-2</v>
       </c>
+      <c r="BU73">
+        <v>1</v>
+      </c>
+      <c r="BV73">
+        <v>0</v>
+      </c>
     </row>
-    <row r="74" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>41401</v>
       </c>
@@ -16733,8 +17178,14 @@
       <c r="BT74" s="12">
         <v>2.5793650793650879E-2</v>
       </c>
+      <c r="BU74">
+        <v>1</v>
+      </c>
+      <c r="BV74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="75" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>41429</v>
       </c>
@@ -16951,8 +17402,14 @@
       <c r="BT75" s="12">
         <v>5.5721393034825817E-2</v>
       </c>
+      <c r="BU75">
+        <v>1</v>
+      </c>
+      <c r="BV75">
+        <v>0</v>
+      </c>
     </row>
-    <row r="76" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>41457</v>
       </c>
@@ -17169,8 +17626,14 @@
       <c r="BT76" s="12">
         <v>5.5721393034825817E-2</v>
       </c>
+      <c r="BU76">
+        <v>1</v>
+      </c>
+      <c r="BV76">
+        <v>0</v>
+      </c>
     </row>
-    <row r="77" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>41492</v>
       </c>
@@ -17387,8 +17850,14 @@
       <c r="BT77" s="12">
         <v>5.5721393034825817E-2</v>
       </c>
+      <c r="BU77">
+        <v>1</v>
+      </c>
+      <c r="BV77">
+        <v>0</v>
+      </c>
     </row>
-    <row r="78" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>41520</v>
       </c>
@@ -17605,8 +18074,14 @@
       <c r="BT78" s="12">
         <v>7.6616915422885595E-2</v>
       </c>
+      <c r="BU78">
+        <v>1</v>
+      </c>
+      <c r="BV78">
+        <v>0</v>
+      </c>
     </row>
-    <row r="79" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>41548</v>
       </c>
@@ -17823,8 +18298,14 @@
       <c r="BT79" s="12">
         <v>7.6616915422885595E-2</v>
       </c>
+      <c r="BU79">
+        <v>1</v>
+      </c>
+      <c r="BV79">
+        <v>0</v>
+      </c>
     </row>
-    <row r="80" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>41583</v>
       </c>
@@ -18041,8 +18522,14 @@
       <c r="BT80" s="12">
         <v>7.6616915422885595E-2</v>
       </c>
+      <c r="BU80">
+        <v>1</v>
+      </c>
+      <c r="BV80">
+        <v>0</v>
+      </c>
     </row>
-    <row r="81" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>41611</v>
       </c>
@@ -18259,8 +18746,14 @@
       <c r="BT81" s="12">
         <v>8.7633885102239531E-2</v>
       </c>
+      <c r="BU81">
+        <v>1</v>
+      </c>
+      <c r="BV81">
+        <v>0</v>
+      </c>
     </row>
-    <row r="82" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>41674</v>
       </c>
@@ -18477,8 +18970,14 @@
       <c r="BT82" s="12">
         <v>8.7633885102239531E-2</v>
       </c>
+      <c r="BU82">
+        <v>1</v>
+      </c>
+      <c r="BV82">
+        <v>0</v>
+      </c>
     </row>
-    <row r="83" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>41702</v>
       </c>
@@ -18695,8 +19194,14 @@
       <c r="BT83" s="12">
         <v>9.9613152804642127E-2</v>
       </c>
+      <c r="BU83">
+        <v>1</v>
+      </c>
+      <c r="BV83">
+        <v>0</v>
+      </c>
     </row>
-    <row r="84" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>41730</v>
       </c>
@@ -18913,8 +19418,14 @@
       <c r="BT84" s="12">
         <v>9.9613152804642127E-2</v>
       </c>
+      <c r="BU84">
+        <v>1</v>
+      </c>
+      <c r="BV84">
+        <v>0</v>
+      </c>
     </row>
-    <row r="85" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>41765</v>
       </c>
@@ -19131,8 +19642,14 @@
       <c r="BT85" s="12">
         <v>9.9613152804642127E-2</v>
       </c>
+      <c r="BU85">
+        <v>1</v>
+      </c>
+      <c r="BV85">
+        <v>0</v>
+      </c>
     </row>
-    <row r="86" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>41793</v>
       </c>
@@ -19349,8 +19866,14 @@
       <c r="BT86" s="12">
         <v>8.859566446748357E-2</v>
       </c>
+      <c r="BU86">
+        <v>1</v>
+      </c>
+      <c r="BV86">
+        <v>0</v>
+      </c>
     </row>
-    <row r="87" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>41821</v>
       </c>
@@ -19567,8 +20090,14 @@
       <c r="BT87" s="12">
         <v>8.859566446748357E-2</v>
       </c>
+      <c r="BU87">
+        <v>1</v>
+      </c>
+      <c r="BV87">
+        <v>0</v>
+      </c>
     </row>
-    <row r="88" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>41856</v>
       </c>
@@ -19785,8 +20314,14 @@
       <c r="BT88" s="12">
         <v>8.859566446748357E-2</v>
       </c>
+      <c r="BU88">
+        <v>1</v>
+      </c>
+      <c r="BV88">
+        <v>0</v>
+      </c>
     </row>
-    <row r="89" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>41884</v>
       </c>
@@ -20003,8 +20538,14 @@
       <c r="BT89" s="12">
         <v>7.3012939001848354E-2</v>
       </c>
+      <c r="BU89">
+        <v>1</v>
+      </c>
+      <c r="BV89">
+        <v>0</v>
+      </c>
     </row>
-    <row r="90" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>41919</v>
       </c>
@@ -20221,8 +20762,14 @@
       <c r="BT90" s="12">
         <v>7.3012939001848354E-2</v>
       </c>
+      <c r="BU90">
+        <v>1</v>
+      </c>
+      <c r="BV90">
+        <v>0</v>
+      </c>
     </row>
-    <row r="91" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>41947</v>
       </c>
@@ -20439,8 +20986,14 @@
       <c r="BT91" s="12">
         <v>7.3012939001848354E-2</v>
       </c>
+      <c r="BU91">
+        <v>1</v>
+      </c>
+      <c r="BV91">
+        <v>0</v>
+      </c>
     </row>
-    <row r="92" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>41975</v>
       </c>
@@ -20657,8 +21210,14 @@
       <c r="BT92" s="12">
         <v>5.9086839749328504E-2</v>
       </c>
+      <c r="BU92">
+        <v>1</v>
+      </c>
+      <c r="BV92">
+        <v>0</v>
+      </c>
     </row>
-    <row r="93" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>42038</v>
       </c>
@@ -20875,8 +21434,14 @@
       <c r="BT93" s="12">
         <v>5.9086839749328504E-2</v>
       </c>
+      <c r="BU93">
+        <v>1</v>
+      </c>
+      <c r="BV93">
+        <v>0</v>
+      </c>
     </row>
-    <row r="94" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>42066</v>
       </c>
@@ -21093,8 +21658,14 @@
       <c r="BT94" s="12">
         <v>4.9252418645558439E-2</v>
       </c>
+      <c r="BU94">
+        <v>1</v>
+      </c>
+      <c r="BV94">
+        <v>0</v>
+      </c>
     </row>
-    <row r="95" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>42101</v>
       </c>
@@ -21311,8 +21882,14 @@
       <c r="BT95" s="12">
         <v>4.9252418645558439E-2</v>
       </c>
+      <c r="BU95">
+        <v>1</v>
+      </c>
+      <c r="BV95">
+        <v>0</v>
+      </c>
     </row>
-    <row r="96" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>42129</v>
       </c>
@@ -21529,8 +22106,14 @@
       <c r="BT96" s="12">
         <v>4.9252418645558439E-2</v>
       </c>
+      <c r="BU96">
+        <v>1</v>
+      </c>
+      <c r="BV96">
+        <v>0</v>
+      </c>
     </row>
-    <row r="97" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>42157</v>
       </c>
@@ -21747,8 +22330,14 @@
       <c r="BT97" s="12">
         <v>7.532467532467535E-2</v>
       </c>
+      <c r="BU97">
+        <v>1</v>
+      </c>
+      <c r="BV97">
+        <v>0</v>
+      </c>
     </row>
-    <row r="98" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>42192</v>
       </c>
@@ -21965,8 +22554,14 @@
       <c r="BT98" s="12">
         <v>7.532467532467535E-2</v>
       </c>
+      <c r="BU98">
+        <v>1</v>
+      </c>
+      <c r="BV98">
+        <v>0</v>
+      </c>
     </row>
-    <row r="99" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>42220</v>
       </c>
@@ -22183,8 +22778,14 @@
       <c r="BT99" s="12">
         <v>7.532467532467535E-2</v>
       </c>
+      <c r="BU99">
+        <v>1</v>
+      </c>
+      <c r="BV99">
+        <v>0</v>
+      </c>
     </row>
-    <row r="100" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>42248</v>
       </c>
@@ -22401,8 +23002,14 @@
       <c r="BT100" s="12">
         <v>8.6993970714901031E-2</v>
       </c>
+      <c r="BU100">
+        <v>1</v>
+      </c>
+      <c r="BV100">
+        <v>0</v>
+      </c>
     </row>
-    <row r="101" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
         <v>42283</v>
       </c>
@@ -22619,8 +23226,14 @@
       <c r="BT101" s="12">
         <v>8.6993970714901031E-2</v>
       </c>
+      <c r="BU101">
+        <v>1</v>
+      </c>
+      <c r="BV101">
+        <v>0</v>
+      </c>
     </row>
-    <row r="102" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
         <v>42311</v>
       </c>
@@ -22837,8 +23450,14 @@
       <c r="BT102" s="12">
         <v>8.6993970714901031E-2</v>
       </c>
+      <c r="BU102">
+        <v>1</v>
+      </c>
+      <c r="BV102">
+        <v>0</v>
+      </c>
     </row>
-    <row r="103" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>42339</v>
       </c>
@@ -23055,8 +23674,14 @@
       <c r="BT103" s="12">
         <v>6.677937447168221E-2</v>
       </c>
+      <c r="BU103">
+        <v>1</v>
+      </c>
+      <c r="BV103">
+        <v>0</v>
+      </c>
     </row>
-    <row r="104" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>42402</v>
       </c>
@@ -23273,8 +23898,14 @@
       <c r="BT104" s="12">
         <v>6.677937447168221E-2</v>
       </c>
+      <c r="BU104">
+        <v>1</v>
+      </c>
+      <c r="BV104">
+        <v>0</v>
+      </c>
     </row>
-    <row r="105" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
         <v>42430</v>
       </c>
@@ -23491,8 +24122,14 @@
       <c r="BT105" s="12">
         <v>4.9455155071249E-2</v>
       </c>
+      <c r="BU105">
+        <v>1</v>
+      </c>
+      <c r="BV105">
+        <v>0</v>
+      </c>
     </row>
-    <row r="106" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>42465</v>
       </c>
@@ -23709,8 +24346,14 @@
       <c r="BT106" s="12">
         <v>4.9455155071249E-2</v>
       </c>
+      <c r="BU106">
+        <v>1</v>
+      </c>
+      <c r="BV106">
+        <v>0</v>
+      </c>
     </row>
-    <row r="107" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
         <v>42493</v>
       </c>
@@ -23927,8 +24570,14 @@
       <c r="BT107" s="12">
         <v>4.9455155071249E-2</v>
       </c>
+      <c r="BU107">
+        <v>1</v>
+      </c>
+      <c r="BV107">
+        <v>0</v>
+      </c>
     </row>
-    <row r="108" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>42528</v>
       </c>
@@ -24145,8 +24794,14 @@
       <c r="BT108" s="12">
         <v>2.1739130434782632E-2</v>
       </c>
+      <c r="BU108">
+        <v>1</v>
+      </c>
+      <c r="BV108">
+        <v>0</v>
+      </c>
     </row>
-    <row r="109" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>42556</v>
       </c>
@@ -24363,8 +25018,14 @@
       <c r="BT109" s="12">
         <v>2.1739130434782632E-2</v>
       </c>
+      <c r="BU109">
+        <v>1</v>
+      </c>
+      <c r="BV109">
+        <v>0</v>
+      </c>
     </row>
-    <row r="110" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>42584</v>
       </c>
@@ -24581,8 +25242,14 @@
       <c r="BT110" s="12">
         <v>2.1739130434782632E-2</v>
       </c>
+      <c r="BU110">
+        <v>1</v>
+      </c>
+      <c r="BV110">
+        <v>0</v>
+      </c>
     </row>
-    <row r="111" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>42619</v>
       </c>
@@ -24799,8 +25466,14 @@
       <c r="BT111" s="12">
         <v>1.7432646592710006E-2</v>
       </c>
+      <c r="BU111">
+        <v>1</v>
+      </c>
+      <c r="BV111">
+        <v>0</v>
+      </c>
     </row>
-    <row r="112" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
         <v>42647</v>
       </c>
@@ -25017,8 +25690,14 @@
       <c r="BT112" s="12">
         <v>1.7432646592710006E-2</v>
       </c>
+      <c r="BU112">
+        <v>0</v>
+      </c>
+      <c r="BV112">
+        <v>1</v>
+      </c>
     </row>
-    <row r="113" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>42675</v>
       </c>
@@ -25235,8 +25914,14 @@
       <c r="BT113" s="12">
         <v>1.7432646592710006E-2</v>
       </c>
+      <c r="BU113">
+        <v>0</v>
+      </c>
+      <c r="BV113">
+        <v>1</v>
+      </c>
     </row>
-    <row r="114" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
         <v>42710</v>
       </c>
@@ -25453,8 +26138,14 @@
       <c r="BT114" s="12">
         <v>4.0412044374009574E-2</v>
       </c>
+      <c r="BU114">
+        <v>0</v>
+      </c>
+      <c r="BV114">
+        <v>1</v>
+      </c>
     </row>
-    <row r="115" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
         <v>42773</v>
       </c>
@@ -25671,8 +26362,14 @@
       <c r="BT115" s="12">
         <v>4.0412044374009574E-2</v>
       </c>
+      <c r="BU115">
+        <v>0</v>
+      </c>
+      <c r="BV115">
+        <v>1</v>
+      </c>
     </row>
-    <row r="116" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A116" s="3">
         <v>42801</v>
       </c>
@@ -25889,8 +26586,14 @@
       <c r="BT116" s="12">
         <v>6.6293929712460037E-2</v>
       </c>
+      <c r="BU116">
+        <v>0</v>
+      </c>
+      <c r="BV116">
+        <v>1</v>
+      </c>
     </row>
-    <row r="117" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A117" s="3">
         <v>42829</v>
       </c>
@@ -26107,8 +26810,14 @@
       <c r="BT117" s="12">
         <v>6.6293929712460037E-2</v>
       </c>
+      <c r="BU117">
+        <v>0</v>
+      </c>
+      <c r="BV117">
+        <v>1</v>
+      </c>
     </row>
-    <row r="118" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A118" s="3">
         <v>42857</v>
       </c>
@@ -26325,8 +27034,14 @@
       <c r="BT118" s="12">
         <v>6.6293929712460037E-2</v>
       </c>
+      <c r="BU118">
+        <v>0</v>
+      </c>
+      <c r="BV118">
+        <v>1</v>
+      </c>
     </row>
-    <row r="119" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
         <v>42892</v>
       </c>
@@ -26543,8 +27258,14 @@
       <c r="BT119" s="12">
         <v>7.2498029944838366E-2</v>
       </c>
+      <c r="BU119">
+        <v>0</v>
+      </c>
+      <c r="BV119">
+        <v>1</v>
+      </c>
     </row>
-    <row r="120" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
         <v>42920</v>
       </c>
@@ -26761,8 +27482,14 @@
       <c r="BT120" s="12">
         <v>7.2498029944838366E-2</v>
       </c>
+      <c r="BU120">
+        <v>0</v>
+      </c>
+      <c r="BV120">
+        <v>1</v>
+      </c>
     </row>
-    <row r="121" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A121" s="3">
         <v>42948</v>
       </c>
@@ -26979,8 +27706,14 @@
       <c r="BT121" s="12">
         <v>7.2498029944838366E-2</v>
       </c>
+      <c r="BU121">
+        <v>0</v>
+      </c>
+      <c r="BV121">
+        <v>1</v>
+      </c>
     </row>
-    <row r="122" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
         <v>42983</v>
       </c>
@@ -27197,8 +27930,14 @@
       <c r="BT122" s="12">
         <v>5.1401869158878455E-2</v>
       </c>
+      <c r="BU122">
+        <v>0</v>
+      </c>
+      <c r="BV122">
+        <v>1</v>
+      </c>
     </row>
-    <row r="123" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
         <v>43011</v>
       </c>
@@ -27415,8 +28154,14 @@
       <c r="BT123" s="12">
         <v>5.1401869158878455E-2</v>
       </c>
+      <c r="BU123">
+        <v>0</v>
+      </c>
+      <c r="BV123">
+        <v>1</v>
+      </c>
     </row>
-    <row r="124" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
         <v>43046</v>
       </c>
@@ -27633,8 +28378,14 @@
       <c r="BT124" s="12">
         <v>5.1401869158878455E-2</v>
       </c>
+      <c r="BU124">
+        <v>0</v>
+      </c>
+      <c r="BV124">
+        <v>1</v>
+      </c>
     </row>
-    <row r="125" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A125" s="3">
         <v>43074</v>
       </c>
@@ -27851,8 +28602,14 @@
       <c r="BT125" s="12">
         <v>3.4272658035034272E-2</v>
       </c>
+      <c r="BU125">
+        <v>0</v>
+      </c>
+      <c r="BV125">
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
         <v>43137</v>
       </c>
@@ -28069,8 +28826,14 @@
       <c r="BT126" s="12">
         <v>3.4272658035034272E-2</v>
       </c>
+      <c r="BU126">
+        <v>0</v>
+      </c>
+      <c r="BV126">
+        <v>1</v>
+      </c>
     </row>
-    <row r="127" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A127" s="3">
         <v>43165</v>
       </c>
@@ -28287,8 +29050,14 @@
       <c r="BT127" s="12">
         <v>1.0486891385767833E-2</v>
       </c>
+      <c r="BU127">
+        <v>0</v>
+      </c>
+      <c r="BV127">
+        <v>1</v>
+      </c>
     </row>
-    <row r="128" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A128" s="3">
         <v>43193</v>
       </c>
@@ -28505,8 +29274,14 @@
       <c r="BT128" s="12">
         <v>1.0486891385767833E-2</v>
       </c>
+      <c r="BU128">
+        <v>0</v>
+      </c>
+      <c r="BV128">
+        <v>1</v>
+      </c>
     </row>
-    <row r="129" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
         <v>43221</v>
       </c>
@@ -28723,8 +29498,14 @@
       <c r="BT129" s="12">
         <v>1.0486891385767833E-2</v>
       </c>
+      <c r="BU129">
+        <v>0</v>
+      </c>
+      <c r="BV129">
+        <v>1</v>
+      </c>
     </row>
-    <row r="130" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
         <v>43256</v>
       </c>
@@ -28941,8 +29722,14 @@
       <c r="BT130" s="12">
         <v>-1.6164584864070453E-2</v>
       </c>
+      <c r="BU130">
+        <v>0</v>
+      </c>
+      <c r="BV130">
+        <v>1</v>
+      </c>
     </row>
-    <row r="131" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A131" s="3">
         <v>43284</v>
       </c>
@@ -29159,8 +29946,14 @@
       <c r="BT131" s="12">
         <v>-1.6164584864070453E-2</v>
       </c>
+      <c r="BU131">
+        <v>0</v>
+      </c>
+      <c r="BV131">
+        <v>1</v>
+      </c>
     </row>
-    <row r="132" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A132" s="3">
         <v>43319</v>
       </c>
@@ -29377,8 +30170,14 @@
       <c r="BT132" s="12">
         <v>-1.6164584864070453E-2</v>
       </c>
+      <c r="BU132">
+        <v>0</v>
+      </c>
+      <c r="BV132">
+        <v>1</v>
+      </c>
     </row>
-    <row r="133" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A133" s="3">
         <v>43347</v>
       </c>
@@ -29595,8 +30394,14 @@
       <c r="BT133" s="12">
         <v>-1.7777777777777819E-2</v>
       </c>
+      <c r="BU133">
+        <v>0</v>
+      </c>
+      <c r="BV133">
+        <v>1</v>
+      </c>
     </row>
-    <row r="134" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A134" s="3">
         <v>43375</v>
       </c>
@@ -29813,8 +30618,14 @@
       <c r="BT134" s="12">
         <v>-1.7777777777777819E-2</v>
       </c>
+      <c r="BU134">
+        <v>0</v>
+      </c>
+      <c r="BV134">
+        <v>1</v>
+      </c>
     </row>
-    <row r="135" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A135" s="3">
         <v>43410</v>
       </c>
@@ -30031,8 +30842,14 @@
       <c r="BT135" s="12">
         <v>-1.7777777777777819E-2</v>
       </c>
+      <c r="BU135">
+        <v>0</v>
+      </c>
+      <c r="BV135">
+        <v>1</v>
+      </c>
     </row>
-    <row r="136" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A136" s="3">
         <v>43438</v>
       </c>
@@ -30249,8 +31066,14 @@
       <c r="BT136" s="12">
         <v>-4.1973490427098796E-2</v>
       </c>
+      <c r="BU136">
+        <v>0</v>
+      </c>
+      <c r="BV136">
+        <v>1</v>
+      </c>
     </row>
-    <row r="137" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A137" s="3">
         <v>43501</v>
       </c>
@@ -30467,8 +31290,14 @@
       <c r="BT137" s="12">
         <v>-4.1973490427098796E-2</v>
       </c>
+      <c r="BU137">
+        <v>0</v>
+      </c>
+      <c r="BV137">
+        <v>1</v>
+      </c>
     </row>
-    <row r="138" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A138" s="3">
         <v>43529</v>
       </c>
@@ -30685,8 +31514,14 @@
       <c r="BT138" s="12">
         <v>-6.4492216456634568E-2</v>
       </c>
+      <c r="BU138">
+        <v>0</v>
+      </c>
+      <c r="BV138">
+        <v>1</v>
+      </c>
     </row>
-    <row r="139" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A139" s="3">
         <v>43557</v>
       </c>
@@ -30903,8 +31738,14 @@
       <c r="BT139" s="12">
         <v>-6.4492216456634568E-2</v>
       </c>
+      <c r="BU139">
+        <v>0</v>
+      </c>
+      <c r="BV139">
+        <v>1</v>
+      </c>
     </row>
-    <row r="140" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A140" s="3">
         <v>43592</v>
       </c>
@@ -31121,8 +31962,14 @@
       <c r="BT140" s="12">
         <v>-6.4492216456634568E-2</v>
       </c>
+      <c r="BU140">
+        <v>0</v>
+      </c>
+      <c r="BV140">
+        <v>1</v>
+      </c>
     </row>
-    <row r="141" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A141" s="3">
         <v>43620</v>
       </c>
@@ -31339,8 +32186,14 @@
       <c r="BT141" s="12">
         <v>-6.4973861090365959E-2</v>
       </c>
+      <c r="BU141">
+        <v>0</v>
+      </c>
+      <c r="BV141">
+        <v>1</v>
+      </c>
     </row>
-    <row r="142" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A142" s="3">
         <v>43648</v>
       </c>
@@ -31557,8 +32410,14 @@
       <c r="BT142" s="12">
         <v>-6.4973861090365959E-2</v>
       </c>
+      <c r="BU142">
+        <v>0</v>
+      </c>
+      <c r="BV142">
+        <v>1</v>
+      </c>
     </row>
-    <row r="143" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A143" s="3">
         <v>43683</v>
       </c>
@@ -31589,8 +32448,14 @@
       <c r="J143">
         <v>2.9254022428083861E-2</v>
       </c>
+      <c r="BU143">
+        <v>0</v>
+      </c>
+      <c r="BV143">
+        <v>1</v>
+      </c>
     </row>
-    <row r="144" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A144" s="3">
         <v>43711</v>
       </c>
@@ -31621,8 +32486,14 @@
       <c r="J144">
         <v>2.2278803309993631E-2</v>
       </c>
+      <c r="BU144">
+        <v>0</v>
+      </c>
+      <c r="BV144">
+        <v>1</v>
+      </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>43739</v>
       </c>
@@ -31653,8 +32524,14 @@
       <c r="J145">
         <v>3.1446540880503138E-2</v>
       </c>
+      <c r="BU145">
+        <v>0</v>
+      </c>
+      <c r="BV145">
+        <v>1</v>
+      </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A146" s="3">
         <v>43774</v>
       </c>
@@ -31685,8 +32562,14 @@
       <c r="J146">
         <v>3.0697674418604649E-2</v>
       </c>
+      <c r="BU146">
+        <v>0</v>
+      </c>
+      <c r="BV146">
+        <v>1</v>
+      </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A147" s="3">
         <v>43802</v>
       </c>
@@ -31717,8 +32600,14 @@
       <c r="J147">
         <v>2.845036319612591E-2</v>
       </c>
+      <c r="BU147">
+        <v>0</v>
+      </c>
+      <c r="BV147">
+        <v>1</v>
+      </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A148" s="3">
         <v>43865</v>
       </c>
@@ -31749,8 +32638,14 @@
       <c r="J148">
         <v>2.1630615640599E-2</v>
       </c>
+      <c r="BU148">
+        <v>0</v>
+      </c>
+      <c r="BV148">
+        <v>1</v>
+      </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A149" s="3">
         <v>43893</v>
       </c>
@@ -31781,8 +32676,14 @@
       <c r="J149">
         <v>2.2113022113022109E-2</v>
       </c>
+      <c r="BU149">
+        <v>0</v>
+      </c>
+      <c r="BV149">
+        <v>1</v>
+      </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A150" s="3">
         <v>43908</v>
       </c>
@@ -31813,8 +32714,14 @@
       <c r="J150">
         <v>2.0242914979757089E-2</v>
       </c>
+      <c r="BU150">
+        <v>0</v>
+      </c>
+      <c r="BV150">
+        <v>1</v>
+      </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A151" s="3">
         <v>43928</v>
       </c>
@@ -31845,8 +32752,14 @@
       <c r="J151">
         <v>1.9555555555555559E-2</v>
       </c>
+      <c r="BU151">
+        <v>0</v>
+      </c>
+      <c r="BV151">
+        <v>1</v>
+      </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A152" s="3">
         <v>43956</v>
       </c>
@@ -31877,8 +32790,14 @@
       <c r="J152">
         <v>2.228303362001564E-2</v>
       </c>
+      <c r="BU152">
+        <v>0</v>
+      </c>
+      <c r="BV152">
+        <v>1</v>
+      </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A153" s="3">
         <v>43984</v>
       </c>
@@ -31909,8 +32828,14 @@
       <c r="J153">
         <v>2.075572112825971E-2</v>
       </c>
+      <c r="BU153">
+        <v>0</v>
+      </c>
+      <c r="BV153">
+        <v>1</v>
+      </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A154" s="3">
         <v>44019</v>
       </c>
@@ -31941,8 +32866,14 @@
       <c r="J154">
         <v>1.95858981533296E-2</v>
       </c>
+      <c r="BU154">
+        <v>0</v>
+      </c>
+      <c r="BV154">
+        <v>1</v>
+      </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A155" s="3">
         <v>44047</v>
       </c>
@@ -31973,8 +32904,14 @@
       <c r="J155">
         <v>2.492729538845035E-2</v>
       </c>
+      <c r="BU155">
+        <v>0</v>
+      </c>
+      <c r="BV155">
+        <v>1</v>
+      </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A156" s="3">
         <v>44075</v>
       </c>
@@ -32005,8 +32942,14 @@
       <c r="J156">
         <v>2.6898734177215191E-2</v>
       </c>
+      <c r="BU156">
+        <v>0</v>
+      </c>
+      <c r="BV156">
+        <v>1</v>
+      </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A157" s="3">
         <v>44110</v>
       </c>
@@ -32037,8 +32980,14 @@
       <c r="J157">
         <v>3.2139577594123052E-2</v>
       </c>
+      <c r="BU157">
+        <v>0</v>
+      </c>
+      <c r="BV157">
+        <v>1</v>
+      </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A158" s="3">
         <v>44138</v>
       </c>
@@ -32069,8 +33018,14 @@
       <c r="J158">
         <v>3.9348710990502037E-2</v>
       </c>
+      <c r="BU158">
+        <v>0</v>
+      </c>
+      <c r="BV158">
+        <v>1</v>
+      </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A159" s="3">
         <v>44166</v>
       </c>
@@ -32101,8 +33056,14 @@
       <c r="J159">
         <v>2.784090909090909E-2</v>
       </c>
+      <c r="BU159">
+        <v>0</v>
+      </c>
+      <c r="BV159">
+        <v>1</v>
+      </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A160" s="3">
         <v>44229</v>
       </c>
@@ -32133,8 +33094,14 @@
       <c r="J160">
         <v>3.7562986715529087E-2</v>
       </c>
+      <c r="BU160">
+        <v>0</v>
+      </c>
+      <c r="BV160">
+        <v>1</v>
+      </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A161" s="3">
         <v>44257</v>
       </c>
@@ -32164,6 +33131,12 @@
       </c>
       <c r="J161">
         <v>3.2531824611032531E-2</v>
+      </c>
+      <c r="BU161">
+        <v>0</v>
+      </c>
+      <c r="BV161">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Australia uncertainty index, playing around with NAIRU estimation as well
</commit_message>
<xml_diff>
--- a/Complied Data.xlsx
+++ b/Complied Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\R-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2503AE-F757-4D8D-ACE2-24FBBA43AAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6251A2-8E64-489D-B0A7-23B0B0B97159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="106">
   <si>
     <t>Dates</t>
   </si>
@@ -398,6 +398,9 @@
   <si>
     <t>Phillip Lowe</t>
   </si>
+  <si>
+    <t>Australia</t>
+  </si>
 </sst>
 </file>
 
@@ -407,7 +410,7 @@
     <numFmt numFmtId="164" formatCode="0.0;\-0.0;0.0;@"/>
     <numFmt numFmtId="165" formatCode="0.00;\-0.00;0.00;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,6 +441,12 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -485,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -516,6 +525,9 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,12 +830,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BV161"/>
+  <dimension ref="A1:BW161"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AT1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="BX15" sqref="BX15"/>
+      <selection pane="bottomLeft" activeCell="BY28" sqref="BY28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -831,7 +843,7 @@
     <col min="1" max="1" width="18.26953125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" ht="71.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:75" ht="71.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1054,8 +1066,11 @@
       <c r="BV1" s="13" t="s">
         <v>104</v>
       </c>
+      <c r="BW1" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="2" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>38993</v>
       </c>
@@ -1266,8 +1281,11 @@
       <c r="BV2">
         <v>0</v>
       </c>
+      <c r="BW2">
+        <v>-1.2663492500002134</v>
+      </c>
     </row>
-    <row r="3" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>39028</v>
       </c>
@@ -1478,8 +1496,11 @@
       <c r="BV3">
         <v>0</v>
       </c>
+      <c r="BW3">
+        <v>-0.91094685139230214</v>
+      </c>
     </row>
-    <row r="4" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>39056</v>
       </c>
@@ -1690,8 +1711,11 @@
       <c r="BV4">
         <v>0</v>
       </c>
+      <c r="BW4">
+        <v>-1.129759307027256</v>
+      </c>
     </row>
-    <row r="5" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>39119</v>
       </c>
@@ -1902,8 +1926,11 @@
       <c r="BV5">
         <v>0</v>
       </c>
+      <c r="BW5">
+        <v>-0.78800506481078281</v>
+      </c>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>39147</v>
       </c>
@@ -2114,8 +2141,11 @@
       <c r="BV6">
         <v>0</v>
       </c>
+      <c r="BW6">
+        <v>-0.79397807957578448</v>
+      </c>
     </row>
-    <row r="7" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>39175</v>
       </c>
@@ -2326,8 +2356,11 @@
       <c r="BV7">
         <v>0</v>
       </c>
+      <c r="BW7">
+        <v>-0.95118664339525094</v>
+      </c>
     </row>
-    <row r="8" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>39203</v>
       </c>
@@ -2538,8 +2571,11 @@
       <c r="BV8">
         <v>0</v>
       </c>
+      <c r="BW8">
+        <v>-0.98911490144087499</v>
+      </c>
     </row>
-    <row r="9" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>39238</v>
       </c>
@@ -2750,8 +2786,11 @@
       <c r="BV9">
         <v>0</v>
       </c>
+      <c r="BW9">
+        <v>-0.61245606709821299</v>
+      </c>
     </row>
-    <row r="10" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>39266</v>
       </c>
@@ -2962,8 +3001,11 @@
       <c r="BV10">
         <v>0</v>
       </c>
+      <c r="BW10">
+        <v>0.41353660114052965</v>
+      </c>
     </row>
-    <row r="11" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>39301</v>
       </c>
@@ -3174,8 +3216,11 @@
       <c r="BV11">
         <v>0</v>
       </c>
+      <c r="BW11">
+        <v>2.2520059976471853</v>
+      </c>
     </row>
-    <row r="12" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>39329</v>
       </c>
@@ -3386,8 +3431,11 @@
       <c r="BV12">
         <v>0</v>
       </c>
+      <c r="BW12">
+        <v>0.39778142810636247</v>
+      </c>
     </row>
-    <row r="13" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>39357</v>
       </c>
@@ -3598,8 +3646,11 @@
       <c r="BV13">
         <v>0</v>
       </c>
+      <c r="BW13">
+        <v>0.57485320823428854</v>
+      </c>
     </row>
-    <row r="14" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>39392</v>
       </c>
@@ -3810,8 +3861,11 @@
       <c r="BV14">
         <v>0</v>
       </c>
+      <c r="BW14">
+        <v>1.6594576651570732</v>
+      </c>
     </row>
-    <row r="15" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>39420</v>
       </c>
@@ -4022,8 +4076,11 @@
       <c r="BV15">
         <v>0</v>
       </c>
+      <c r="BW15">
+        <v>0.33186667875239129</v>
+      </c>
     </row>
-    <row r="16" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>39483</v>
       </c>
@@ -4234,8 +4291,11 @@
       <c r="BV16">
         <v>0</v>
       </c>
+      <c r="BW16">
+        <v>0.97209611605705981</v>
+      </c>
     </row>
-    <row r="17" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>39511</v>
       </c>
@@ -4446,8 +4506,11 @@
       <c r="BV17">
         <v>0</v>
       </c>
+      <c r="BW17">
+        <v>1.6904551387487603</v>
+      </c>
     </row>
-    <row r="18" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>39539</v>
       </c>
@@ -4658,8 +4721,11 @@
       <c r="BV18">
         <v>0</v>
       </c>
+      <c r="BW18">
+        <v>0.51884103355454014</v>
+      </c>
     </row>
-    <row r="19" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>39574</v>
       </c>
@@ -4879,8 +4945,11 @@
       <c r="BV19">
         <v>0</v>
       </c>
+      <c r="BW19">
+        <v>-3.127336555252818E-2</v>
+      </c>
     </row>
-    <row r="20" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>39602</v>
       </c>
@@ -5100,8 +5169,11 @@
       <c r="BV20">
         <v>0</v>
       </c>
+      <c r="BW20">
+        <v>-0.14084174476233274</v>
+      </c>
     </row>
-    <row r="21" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>39630</v>
       </c>
@@ -5321,8 +5393,11 @@
       <c r="BV21">
         <v>0</v>
       </c>
+      <c r="BW21">
+        <v>0.91750983363553906</v>
+      </c>
     </row>
-    <row r="22" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>39665</v>
       </c>
@@ -5542,8 +5617,11 @@
       <c r="BV22">
         <v>0</v>
       </c>
+      <c r="BW22">
+        <v>1.7304153524781551</v>
+      </c>
     </row>
-    <row r="23" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>39693</v>
       </c>
@@ -5763,8 +5841,11 @@
       <c r="BV23">
         <v>0</v>
       </c>
+      <c r="BW23">
+        <v>5.3325080316419387</v>
+      </c>
     </row>
-    <row r="24" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>39728</v>
       </c>
@@ -5984,8 +6065,11 @@
       <c r="BV24">
         <v>0</v>
       </c>
+      <c r="BW24">
+        <v>11.149727446678112</v>
+      </c>
     </row>
-    <row r="25" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>39756</v>
       </c>
@@ -6208,8 +6292,11 @@
       <c r="BV25">
         <v>0</v>
       </c>
+      <c r="BW25">
+        <v>8.312845593438869</v>
+      </c>
     </row>
-    <row r="26" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>39784</v>
       </c>
@@ -6432,8 +6519,11 @@
       <c r="BV26">
         <v>0</v>
       </c>
+      <c r="BW26">
+        <v>4.3568263505047513</v>
+      </c>
     </row>
-    <row r="27" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>39847</v>
       </c>
@@ -6656,8 +6746,11 @@
       <c r="BV27">
         <v>0</v>
       </c>
+      <c r="BW27">
+        <v>3.3115231920685035</v>
+      </c>
     </row>
-    <row r="28" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>39875</v>
       </c>
@@ -6880,8 +6973,11 @@
       <c r="BV28">
         <v>0</v>
       </c>
+      <c r="BW28">
+        <v>3.0873710488176549</v>
+      </c>
     </row>
-    <row r="29" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>39910</v>
       </c>
@@ -7104,8 +7200,11 @@
       <c r="BV29">
         <v>0</v>
       </c>
+      <c r="BW29">
+        <v>2.3585863439830903</v>
+      </c>
     </row>
-    <row r="30" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>39938</v>
       </c>
@@ -7328,8 +7427,11 @@
       <c r="BV30">
         <v>0</v>
       </c>
+      <c r="BW30">
+        <v>2.2333297809686385</v>
+      </c>
     </row>
-    <row r="31" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>39966</v>
       </c>
@@ -7552,8 +7654,11 @@
       <c r="BV31">
         <v>0</v>
       </c>
+      <c r="BW31">
+        <v>2.4324929102499486</v>
+      </c>
     </row>
-    <row r="32" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>40001</v>
       </c>
@@ -7776,8 +7881,11 @@
       <c r="BV32">
         <v>0</v>
       </c>
+      <c r="BW32">
+        <v>1.6795427410855193</v>
+      </c>
     </row>
-    <row r="33" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>40029</v>
       </c>
@@ -8000,8 +8108,11 @@
       <c r="BV33">
         <v>0</v>
       </c>
+      <c r="BW33">
+        <v>0.45463356551528977</v>
+      </c>
     </row>
-    <row r="34" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>40057</v>
       </c>
@@ -8224,8 +8335,11 @@
       <c r="BV34">
         <v>0</v>
       </c>
+      <c r="BW34">
+        <v>0.72052826134948245</v>
+      </c>
     </row>
-    <row r="35" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>40092</v>
       </c>
@@ -8448,8 +8562,11 @@
       <c r="BV35">
         <v>0</v>
       </c>
+      <c r="BW35">
+        <v>1.0950481648377159</v>
+      </c>
     </row>
-    <row r="36" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>40120</v>
       </c>
@@ -8672,8 +8789,11 @@
       <c r="BV36">
         <v>0</v>
       </c>
+      <c r="BW36">
+        <v>0.87422278620440375</v>
+      </c>
     </row>
-    <row r="37" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>40148</v>
       </c>
@@ -8896,8 +9016,11 @@
       <c r="BV37">
         <v>0</v>
       </c>
+      <c r="BW37">
+        <v>0.57706867370594916</v>
+      </c>
     </row>
-    <row r="38" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>40211</v>
       </c>
@@ -9120,8 +9243,11 @@
       <c r="BV38">
         <v>0</v>
       </c>
+      <c r="BW38">
+        <v>0.22993517510814637</v>
+      </c>
     </row>
-    <row r="39" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>40239</v>
       </c>
@@ -9344,8 +9470,11 @@
       <c r="BV39">
         <v>0</v>
       </c>
+      <c r="BW39">
+        <v>-0.17296483463475798</v>
+      </c>
     </row>
-    <row r="40" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>40274</v>
       </c>
@@ -9568,8 +9697,11 @@
       <c r="BV40">
         <v>0</v>
       </c>
+      <c r="BW40">
+        <v>-0.23520811583116955</v>
+      </c>
     </row>
-    <row r="41" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>40302</v>
       </c>
@@ -9792,8 +9924,11 @@
       <c r="BV41">
         <v>0</v>
       </c>
+      <c r="BW41">
+        <v>2.8202782752416327</v>
+      </c>
     </row>
-    <row r="42" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>40330</v>
       </c>
@@ -10016,8 +10151,11 @@
       <c r="BV42">
         <v>0</v>
       </c>
+      <c r="BW42">
+        <v>2.1645268099327124</v>
+      </c>
     </row>
-    <row r="43" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>40365</v>
       </c>
@@ -10240,8 +10378,11 @@
       <c r="BV43">
         <v>0</v>
       </c>
+      <c r="BW43">
+        <v>1.3660483699086154</v>
+      </c>
     </row>
-    <row r="44" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>40393</v>
       </c>
@@ -10464,8 +10605,11 @@
       <c r="BV44">
         <v>0</v>
       </c>
+      <c r="BW44">
+        <v>0.33612165615405465</v>
+      </c>
     </row>
-    <row r="45" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>40428</v>
       </c>
@@ -10688,8 +10832,11 @@
       <c r="BV45">
         <v>0</v>
       </c>
+      <c r="BW45">
+        <v>4.5776873695923828E-2</v>
+      </c>
     </row>
-    <row r="46" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>40456</v>
       </c>
@@ -10912,8 +11059,11 @@
       <c r="BV46">
         <v>0</v>
       </c>
+      <c r="BW46">
+        <v>0.82130203465062745</v>
+      </c>
     </row>
-    <row r="47" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>40484</v>
       </c>
@@ -11136,8 +11286,11 @@
       <c r="BV47">
         <v>0</v>
       </c>
+      <c r="BW47">
+        <v>0.53850940958329307</v>
+      </c>
     </row>
-    <row r="48" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>40519</v>
       </c>
@@ -11360,8 +11513,11 @@
       <c r="BV48">
         <v>0</v>
       </c>
+      <c r="BW48">
+        <v>2.7977835017245815E-2</v>
+      </c>
     </row>
-    <row r="49" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>40575</v>
       </c>
@@ -11584,8 +11740,11 @@
       <c r="BV49">
         <v>0</v>
       </c>
+      <c r="BW49">
+        <v>-0.46516663059357377</v>
+      </c>
     </row>
-    <row r="50" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>40603</v>
       </c>
@@ -11808,8 +11967,11 @@
       <c r="BV50">
         <v>0</v>
       </c>
+      <c r="BW50">
+        <v>6.8191338296916121E-2</v>
+      </c>
     </row>
-    <row r="51" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>40638</v>
       </c>
@@ -12032,8 +12194,11 @@
       <c r="BV51">
         <v>0</v>
       </c>
+      <c r="BW51">
+        <v>-9.6688870158054552E-3</v>
+      </c>
     </row>
-    <row r="52" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>40666</v>
       </c>
@@ -12256,8 +12421,11 @@
       <c r="BV52">
         <v>0</v>
       </c>
+      <c r="BW52">
+        <v>0.47256484508407159</v>
+      </c>
     </row>
-    <row r="53" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>40701</v>
       </c>
@@ -12480,8 +12648,11 @@
       <c r="BV53">
         <v>0</v>
       </c>
+      <c r="BW53">
+        <v>0.19458155116834408</v>
+      </c>
     </row>
-    <row r="54" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>40729</v>
       </c>
@@ -12704,8 +12875,11 @@
       <c r="BV54">
         <v>0</v>
       </c>
+      <c r="BW54">
+        <v>0.40109932264902992</v>
+      </c>
     </row>
-    <row r="55" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>40757</v>
       </c>
@@ -12928,8 +13102,11 @@
       <c r="BV55">
         <v>0</v>
       </c>
+      <c r="BW55">
+        <v>1.4377995935801671</v>
+      </c>
     </row>
-    <row r="56" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>40792</v>
       </c>
@@ -13152,8 +13329,11 @@
       <c r="BV56">
         <v>0</v>
       </c>
+      <c r="BW56">
+        <v>2.4297263878368178</v>
+      </c>
     </row>
-    <row r="57" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>40820</v>
       </c>
@@ -13376,8 +13556,11 @@
       <c r="BV57">
         <v>0</v>
       </c>
+      <c r="BW57">
+        <v>2.8319286701435433</v>
+      </c>
     </row>
-    <row r="58" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>40848</v>
       </c>
@@ -13600,8 +13783,11 @@
       <c r="BV58">
         <v>0</v>
       </c>
+      <c r="BW58">
+        <v>2.1224741745633771</v>
+      </c>
     </row>
-    <row r="59" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>40883</v>
       </c>
@@ -13824,8 +14010,11 @@
       <c r="BV59">
         <v>0</v>
       </c>
+      <c r="BW59">
+        <v>1.0297482149509836</v>
+      </c>
     </row>
-    <row r="60" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>40946</v>
       </c>
@@ -14048,8 +14237,11 @@
       <c r="BV60">
         <v>0</v>
       </c>
+      <c r="BW60">
+        <v>-0.10029466481930566</v>
+      </c>
     </row>
-    <row r="61" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>40974</v>
       </c>
@@ -14272,8 +14464,11 @@
       <c r="BV61">
         <v>0</v>
       </c>
+      <c r="BW61">
+        <v>-0.18059546114994426</v>
+      </c>
     </row>
-    <row r="62" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>41002</v>
       </c>
@@ -14496,8 +14691,11 @@
       <c r="BV62">
         <v>0</v>
       </c>
+      <c r="BW62">
+        <v>-0.20539480321421744</v>
+      </c>
     </row>
-    <row r="63" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>41030</v>
       </c>
@@ -14720,8 +14918,11 @@
       <c r="BV63">
         <v>0</v>
       </c>
+      <c r="BW63">
+        <v>0.34458299617836652</v>
+      </c>
     </row>
-    <row r="64" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>41065</v>
       </c>
@@ -14944,8 +15145,11 @@
       <c r="BV64">
         <v>0</v>
       </c>
+      <c r="BW64">
+        <v>0.27624618097096676</v>
+      </c>
     </row>
-    <row r="65" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>41093</v>
       </c>
@@ -15168,8 +15372,11 @@
       <c r="BV65">
         <v>0</v>
       </c>
+      <c r="BW65">
+        <v>-7.3768692721364326E-2</v>
+      </c>
     </row>
-    <row r="66" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>41128</v>
       </c>
@@ -15392,8 +15599,11 @@
       <c r="BV66">
         <v>0</v>
       </c>
+      <c r="BW66">
+        <v>-1.2767421793276204</v>
+      </c>
     </row>
-    <row r="67" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>41156</v>
       </c>
@@ -15616,8 +15826,11 @@
       <c r="BV67">
         <v>0</v>
       </c>
+      <c r="BW67">
+        <v>-0.45109458263377489</v>
+      </c>
     </row>
-    <row r="68" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>41184</v>
       </c>
@@ -15840,8 +16053,11 @@
       <c r="BV68">
         <v>0</v>
       </c>
+      <c r="BW68">
+        <v>-0.76970590733468436</v>
+      </c>
     </row>
-    <row r="69" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>41219</v>
       </c>
@@ -16064,8 +16280,11 @@
       <c r="BV69">
         <v>0</v>
       </c>
+      <c r="BW69">
+        <v>-1.0382312159876297</v>
+      </c>
     </row>
-    <row r="70" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>41247</v>
       </c>
@@ -16288,8 +16507,11 @@
       <c r="BV70">
         <v>0</v>
       </c>
+      <c r="BW70">
+        <v>-1.0691549899203683</v>
+      </c>
     </row>
-    <row r="71" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>41310</v>
       </c>
@@ -16512,8 +16734,11 @@
       <c r="BV71">
         <v>0</v>
       </c>
+      <c r="BW71">
+        <v>-0.96047161160416683</v>
+      </c>
     </row>
-    <row r="72" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>41338</v>
       </c>
@@ -16736,8 +16961,11 @@
       <c r="BV72">
         <v>0</v>
       </c>
+      <c r="BW72">
+        <v>-0.70954627657163893</v>
+      </c>
     </row>
-    <row r="73" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>41366</v>
       </c>
@@ -16960,8 +17188,11 @@
       <c r="BV73">
         <v>0</v>
       </c>
+      <c r="BW73">
+        <v>-0.77330867339775899</v>
+      </c>
     </row>
-    <row r="74" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>41401</v>
       </c>
@@ -17184,8 +17415,11 @@
       <c r="BV74">
         <v>0</v>
       </c>
+      <c r="BW74">
+        <v>-9.225490200552959E-2</v>
+      </c>
     </row>
-    <row r="75" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>41429</v>
       </c>
@@ -17408,8 +17642,11 @@
       <c r="BV75">
         <v>0</v>
       </c>
+      <c r="BW75">
+        <v>1.429682361350388</v>
+      </c>
     </row>
-    <row r="76" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>41457</v>
       </c>
@@ -17632,8 +17869,11 @@
       <c r="BV76">
         <v>0</v>
       </c>
+      <c r="BW76">
+        <v>0.53303871280371062</v>
+      </c>
     </row>
-    <row r="77" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>41492</v>
       </c>
@@ -17856,8 +18096,11 @@
       <c r="BV77">
         <v>0</v>
       </c>
+      <c r="BW77">
+        <v>-0.34914561334149508</v>
+      </c>
     </row>
-    <row r="78" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>41520</v>
       </c>
@@ -18080,8 +18323,11 @@
       <c r="BV78">
         <v>0</v>
       </c>
+      <c r="BW78">
+        <v>-4.9763603132906897E-2</v>
+      </c>
     </row>
-    <row r="79" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>41548</v>
       </c>
@@ -18304,8 +18550,11 @@
       <c r="BV79">
         <v>0</v>
       </c>
+      <c r="BW79">
+        <v>-0.99395764929258679</v>
+      </c>
     </row>
-    <row r="80" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>41583</v>
       </c>
@@ -18528,8 +18777,11 @@
       <c r="BV80">
         <v>0</v>
       </c>
+      <c r="BW80">
+        <v>-0.79119066738725818</v>
+      </c>
     </row>
-    <row r="81" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>41611</v>
       </c>
@@ -18752,8 +19004,11 @@
       <c r="BV81">
         <v>0</v>
       </c>
+      <c r="BW81">
+        <v>-0.26807106559766014</v>
+      </c>
     </row>
-    <row r="82" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>41674</v>
       </c>
@@ -18976,8 +19231,11 @@
       <c r="BV82">
         <v>0</v>
       </c>
+      <c r="BW82">
+        <v>-0.77230749428669576</v>
+      </c>
     </row>
-    <row r="83" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>41702</v>
       </c>
@@ -19200,8 +19458,11 @@
       <c r="BV83">
         <v>0</v>
       </c>
+      <c r="BW83">
+        <v>-1.0454187375232133</v>
+      </c>
     </row>
-    <row r="84" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>41730</v>
       </c>
@@ -19424,8 +19685,11 @@
       <c r="BV84">
         <v>0</v>
       </c>
+      <c r="BW84">
+        <v>-1.1743818249038418</v>
+      </c>
     </row>
-    <row r="85" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>41765</v>
       </c>
@@ -19648,8 +19912,11 @@
       <c r="BV85">
         <v>0</v>
       </c>
+      <c r="BW85">
+        <v>-1.5508134352639837</v>
+      </c>
     </row>
-    <row r="86" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>41793</v>
       </c>
@@ -19872,8 +20139,11 @@
       <c r="BV86">
         <v>0</v>
       </c>
+      <c r="BW86">
+        <v>-1.1300001587331132</v>
+      </c>
     </row>
-    <row r="87" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>41821</v>
       </c>
@@ -20096,8 +20366,11 @@
       <c r="BV87">
         <v>0</v>
       </c>
+      <c r="BW87">
+        <v>-1.3931230306185229</v>
+      </c>
     </row>
-    <row r="88" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>41856</v>
       </c>
@@ -20320,8 +20593,11 @@
       <c r="BV88">
         <v>0</v>
       </c>
+      <c r="BW88">
+        <v>-1.7407262245088444</v>
+      </c>
     </row>
-    <row r="89" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>41884</v>
       </c>
@@ -20544,8 +20820,11 @@
       <c r="BV89">
         <v>0</v>
       </c>
+      <c r="BW89">
+        <v>-0.83052999169924391</v>
+      </c>
     </row>
-    <row r="90" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>41919</v>
       </c>
@@ -20768,8 +21047,11 @@
       <c r="BV90">
         <v>0</v>
       </c>
+      <c r="BW90">
+        <v>0.38089997502388567</v>
+      </c>
     </row>
-    <row r="91" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>41947</v>
       </c>
@@ -20992,8 +21274,11 @@
       <c r="BV91">
         <v>0</v>
       </c>
+      <c r="BW91">
+        <v>-0.21181719930168139</v>
+      </c>
     </row>
-    <row r="92" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>41975</v>
       </c>
@@ -21216,8 +21501,11 @@
       <c r="BV92">
         <v>0</v>
       </c>
+      <c r="BW92">
+        <v>-0.42375822274849562</v>
+      </c>
     </row>
-    <row r="93" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>42038</v>
       </c>
@@ -21440,8 +21728,11 @@
       <c r="BV93">
         <v>0</v>
       </c>
+      <c r="BW93">
+        <v>0.14144336856195924</v>
+      </c>
     </row>
-    <row r="94" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>42066</v>
       </c>
@@ -21664,8 +21955,11 @@
       <c r="BV94">
         <v>0</v>
       </c>
+      <c r="BW94">
+        <v>0.58721702514918594</v>
+      </c>
     </row>
-    <row r="95" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>42101</v>
       </c>
@@ -21888,8 +22182,11 @@
       <c r="BV95">
         <v>0</v>
       </c>
+      <c r="BW95">
+        <v>0.8045014029894435</v>
+      </c>
     </row>
-    <row r="96" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>42129</v>
       </c>
@@ -22112,8 +22409,11 @@
       <c r="BV96">
         <v>0</v>
       </c>
+      <c r="BW96">
+        <v>0.61999475822219063</v>
+      </c>
     </row>
-    <row r="97" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>42157</v>
       </c>
@@ -22336,8 +22636,11 @@
       <c r="BV97">
         <v>0</v>
       </c>
+      <c r="BW97">
+        <v>1.0396898135548642</v>
+      </c>
     </row>
-    <row r="98" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>42192</v>
       </c>
@@ -22560,8 +22863,11 @@
       <c r="BV98">
         <v>0</v>
       </c>
+      <c r="BW98">
+        <v>0.46805242216488696</v>
+      </c>
     </row>
-    <row r="99" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>42220</v>
       </c>
@@ -22784,8 +23090,11 @@
       <c r="BV99">
         <v>0</v>
       </c>
+      <c r="BW99">
+        <v>1.1711431119292752</v>
+      </c>
     </row>
-    <row r="100" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>42248</v>
       </c>
@@ -23008,8 +23317,11 @@
       <c r="BV100">
         <v>0</v>
       </c>
+      <c r="BW100">
+        <v>0.85892073407507397</v>
+      </c>
     </row>
-    <row r="101" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
         <v>42283</v>
       </c>
@@ -23232,8 +23544,11 @@
       <c r="BV101">
         <v>0</v>
       </c>
+      <c r="BW101">
+        <v>0.61130418598698966</v>
+      </c>
     </row>
-    <row r="102" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
         <v>42311</v>
       </c>
@@ -23456,8 +23771,11 @@
       <c r="BV102">
         <v>0</v>
       </c>
+      <c r="BW102">
+        <v>0.1043160820084562</v>
+      </c>
     </row>
-    <row r="103" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>42339</v>
       </c>
@@ -23680,8 +23998,11 @@
       <c r="BV103">
         <v>0</v>
       </c>
+      <c r="BW103">
+        <v>0.44901894913785312</v>
+      </c>
     </row>
-    <row r="104" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>42402</v>
       </c>
@@ -23904,8 +24225,11 @@
       <c r="BV104">
         <v>0</v>
       </c>
+      <c r="BW104">
+        <v>0.90016752843532555</v>
+      </c>
     </row>
-    <row r="105" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
         <v>42430</v>
       </c>
@@ -24128,8 +24452,11 @@
       <c r="BV105">
         <v>0</v>
       </c>
+      <c r="BW105">
+        <v>0.74728202422074796</v>
+      </c>
     </row>
-    <row r="106" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>42465</v>
       </c>
@@ -24352,8 +24679,11 @@
       <c r="BV106">
         <v>0</v>
       </c>
+      <c r="BW106">
+        <v>0.66344356806211857</v>
+      </c>
     </row>
-    <row r="107" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
         <v>42493</v>
       </c>
@@ -24576,8 +24906,11 @@
       <c r="BV107">
         <v>0</v>
       </c>
+      <c r="BW107">
+        <v>-9.2750473399227651E-3</v>
+      </c>
     </row>
-    <row r="108" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>42528</v>
       </c>
@@ -24800,8 +25133,11 @@
       <c r="BV108">
         <v>0</v>
       </c>
+      <c r="BW108">
+        <v>0.42211660747653029</v>
+      </c>
     </row>
-    <row r="109" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>42556</v>
       </c>
@@ -25024,8 +25360,11 @@
       <c r="BV109">
         <v>0</v>
       </c>
+      <c r="BW109">
+        <v>-3.6724543545708546E-2</v>
+      </c>
     </row>
-    <row r="110" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>42584</v>
       </c>
@@ -25248,8 +25587,11 @@
       <c r="BV110">
         <v>0</v>
       </c>
+      <c r="BW110">
+        <v>-0.7446073454066322</v>
+      </c>
     </row>
-    <row r="111" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>42619</v>
       </c>
@@ -25472,8 +25814,11 @@
       <c r="BV111">
         <v>0</v>
       </c>
+      <c r="BW111">
+        <v>-0.54693226120496807</v>
+      </c>
     </row>
-    <row r="112" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
         <v>42647</v>
       </c>
@@ -25696,8 +26041,11 @@
       <c r="BV112">
         <v>1</v>
       </c>
+      <c r="BW112">
+        <v>-0.33796159994814196</v>
+      </c>
     </row>
-    <row r="113" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>42675</v>
       </c>
@@ -25920,8 +26268,11 @@
       <c r="BV113">
         <v>1</v>
       </c>
+      <c r="BW113">
+        <v>1.5875206014947144E-2</v>
+      </c>
     </row>
-    <row r="114" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
         <v>42710</v>
       </c>
@@ -26144,8 +26495,11 @@
       <c r="BV114">
         <v>1</v>
       </c>
+      <c r="BW114">
+        <v>3.2792211301270691E-2</v>
+      </c>
     </row>
-    <row r="115" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
         <v>42773</v>
       </c>
@@ -26368,8 +26722,11 @@
       <c r="BV115">
         <v>1</v>
       </c>
+      <c r="BW115">
+        <v>-0.44395303222040361</v>
+      </c>
     </row>
-    <row r="116" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A116" s="3">
         <v>42801</v>
       </c>
@@ -26592,8 +26949,11 @@
       <c r="BV116">
         <v>1</v>
       </c>
+      <c r="BW116">
+        <v>-0.53658075720857112</v>
+      </c>
     </row>
-    <row r="117" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A117" s="3">
         <v>42829</v>
       </c>
@@ -26816,8 +27176,11 @@
       <c r="BV117">
         <v>1</v>
       </c>
+      <c r="BW117">
+        <v>-0.43272705073049655</v>
+      </c>
     </row>
-    <row r="118" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A118" s="3">
         <v>42857</v>
       </c>
@@ -27040,8 +27403,11 @@
       <c r="BV118">
         <v>1</v>
       </c>
+      <c r="BW118">
+        <v>-0.93471294926599402</v>
+      </c>
     </row>
-    <row r="119" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
         <v>42892</v>
       </c>
@@ -27264,8 +27630,11 @@
       <c r="BV119">
         <v>1</v>
       </c>
+      <c r="BW119">
+        <v>-1.0766882001500206</v>
+      </c>
     </row>
-    <row r="120" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
         <v>42920</v>
       </c>
@@ -27488,8 +27857,11 @@
       <c r="BV120">
         <v>1</v>
       </c>
+      <c r="BW120">
+        <v>-0.74941294741662756</v>
+      </c>
     </row>
-    <row r="121" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A121" s="3">
         <v>42948</v>
       </c>
@@ -27712,8 +28084,11 @@
       <c r="BV121">
         <v>1</v>
       </c>
+      <c r="BW121">
+        <v>-0.97049854873126673</v>
+      </c>
     </row>
-    <row r="122" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
         <v>42983</v>
       </c>
@@ -27936,8 +28311,11 @@
       <c r="BV122">
         <v>1</v>
       </c>
+      <c r="BW122">
+        <v>-0.58175274844657321</v>
+      </c>
     </row>
-    <row r="123" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
         <v>43011</v>
       </c>
@@ -28160,8 +28538,11 @@
       <c r="BV123">
         <v>1</v>
       </c>
+      <c r="BW123">
+        <v>-0.99812552887574668</v>
+      </c>
     </row>
-    <row r="124" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
         <v>43046</v>
       </c>
@@ -28384,8 +28765,11 @@
       <c r="BV124">
         <v>1</v>
       </c>
+      <c r="BW124">
+        <v>-1.0440056540037357</v>
+      </c>
     </row>
-    <row r="125" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A125" s="3">
         <v>43074</v>
       </c>
@@ -28608,8 +28992,11 @@
       <c r="BV125">
         <v>1</v>
       </c>
+      <c r="BW125">
+        <v>-1.207502971468339</v>
+      </c>
     </row>
-    <row r="126" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
         <v>43137</v>
       </c>
@@ -28832,8 +29219,11 @@
       <c r="BV126">
         <v>1</v>
       </c>
+      <c r="BW126">
+        <v>-0.99501938466764284</v>
+      </c>
     </row>
-    <row r="127" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A127" s="3">
         <v>43165</v>
       </c>
@@ -29056,8 +29446,11 @@
       <c r="BV127">
         <v>1</v>
       </c>
+      <c r="BW127">
+        <v>-0.83150851414681559</v>
+      </c>
     </row>
-    <row r="128" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A128" s="3">
         <v>43193</v>
       </c>
@@ -29280,8 +29673,11 @@
       <c r="BV128">
         <v>1</v>
       </c>
+      <c r="BW128">
+        <v>-1.0965271578713787</v>
+      </c>
     </row>
-    <row r="129" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
         <v>43221</v>
       </c>
@@ -29504,8 +29900,11 @@
       <c r="BV129">
         <v>1</v>
       </c>
+      <c r="BW129">
+        <v>-0.62396258713061203</v>
+      </c>
     </row>
-    <row r="130" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
         <v>43256</v>
       </c>
@@ -29728,8 +30127,11 @@
       <c r="BV130">
         <v>1</v>
       </c>
+      <c r="BW130">
+        <v>-0.58141186469916817</v>
+      </c>
     </row>
-    <row r="131" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A131" s="3">
         <v>43284</v>
       </c>
@@ -29952,8 +30354,11 @@
       <c r="BV131">
         <v>1</v>
       </c>
+      <c r="BW131">
+        <v>-0.70067066667657374</v>
+      </c>
     </row>
-    <row r="132" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A132" s="3">
         <v>43319</v>
       </c>
@@ -30176,8 +30581,11 @@
       <c r="BV132">
         <v>1</v>
       </c>
+      <c r="BW132">
+        <v>-0.80737065477634207</v>
+      </c>
     </row>
-    <row r="133" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A133" s="3">
         <v>43347</v>
       </c>
@@ -30400,8 +30808,11 @@
       <c r="BV133">
         <v>1</v>
       </c>
+      <c r="BW133">
+        <v>-0.74385921393006948</v>
+      </c>
     </row>
-    <row r="134" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A134" s="3">
         <v>43375</v>
       </c>
@@ -30624,8 +31035,11 @@
       <c r="BV134">
         <v>1</v>
       </c>
+      <c r="BW134">
+        <v>-0.51363143036526893</v>
+      </c>
     </row>
-    <row r="135" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A135" s="3">
         <v>43410</v>
       </c>
@@ -30848,8 +31262,11 @@
       <c r="BV135">
         <v>1</v>
       </c>
+      <c r="BW135">
+        <v>-0.67156118276538002</v>
+      </c>
     </row>
-    <row r="136" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A136" s="3">
         <v>43438</v>
       </c>
@@ -31072,8 +31489,11 @@
       <c r="BV136">
         <v>1</v>
       </c>
+      <c r="BW136">
+        <v>-0.69057617786636172</v>
+      </c>
     </row>
-    <row r="137" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A137" s="3">
         <v>43501</v>
       </c>
@@ -31296,8 +31716,11 @@
       <c r="BV137">
         <v>1</v>
       </c>
+      <c r="BW137">
+        <v>-0.83298215442536894</v>
+      </c>
     </row>
-    <row r="138" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A138" s="3">
         <v>43529</v>
       </c>
@@ -31520,8 +31943,11 @@
       <c r="BV138">
         <v>1</v>
       </c>
+      <c r="BW138">
+        <v>-0.84054855789717453</v>
+      </c>
     </row>
-    <row r="139" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A139" s="3">
         <v>43557</v>
       </c>
@@ -31744,8 +32170,11 @@
       <c r="BV139">
         <v>1</v>
       </c>
+      <c r="BW139">
+        <v>-1.1689704636540637</v>
+      </c>
     </row>
-    <row r="140" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A140" s="3">
         <v>43592</v>
       </c>
@@ -31968,8 +32397,11 @@
       <c r="BV140">
         <v>1</v>
       </c>
+      <c r="BW140">
+        <v>-1.4040905621341593</v>
+      </c>
     </row>
-    <row r="141" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A141" s="3">
         <v>43620</v>
       </c>
@@ -32192,8 +32624,11 @@
       <c r="BV141">
         <v>1</v>
       </c>
+      <c r="BW141">
+        <v>-1.0598258834903564</v>
+      </c>
     </row>
-    <row r="142" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A142" s="3">
         <v>43648</v>
       </c>
@@ -32416,8 +32851,11 @@
       <c r="BV142">
         <v>1</v>
       </c>
+      <c r="BW142">
+        <v>-1.1556797599863786</v>
+      </c>
     </row>
-    <row r="143" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A143" s="3">
         <v>43683</v>
       </c>
@@ -32455,7 +32893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A144" s="3">
         <v>43711</v>
       </c>

</xml_diff>

<commit_message>
Trying out specifications with different variables
</commit_message>
<xml_diff>
--- a/Complied Data.xlsx
+++ b/Complied Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\R-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6251A2-8E64-489D-B0A7-23B0B0B97159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEAC285-C6C6-4D9E-AFA2-5362FAAD41ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -545,6 +545,3791 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>sheet1!$AB$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fccpiiq4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>sheet1!$A$2:$A$161</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="160"/>
+                <c:pt idx="0">
+                  <c:v>38993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39056</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39119</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39147</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39175</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39203</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39238</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39266</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39301</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39329</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39357</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39392</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39420</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39483</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39511</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>39539</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39574</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39602</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39630</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39665</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>39693</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>39728</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>39756</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>39784</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39847</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>39875</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>39910</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>39938</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39966</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40029</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40092</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>40120</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40148</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40211</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>40239</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>40274</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40302</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40330</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>40365</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>40393</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>40428</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>40456</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>40484</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>40519</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>40575</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>40603</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>40638</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>40666</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>40701</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>40729</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>40757</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>40792</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>40820</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>40848</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>40883</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>40946</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>40974</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>41002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>41030</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>41065</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>41093</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>41128</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>41156</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>41184</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>41219</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>41247</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>41310</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>41338</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>41366</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>41401</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>41429</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>41457</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>41492</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>41520</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>41548</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>41583</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>41611</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>41674</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>41702</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>41730</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>41765</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>41793</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>41821</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>41856</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>41884</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>41919</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>41947</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>41975</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>42038</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>42066</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>42101</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>42129</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>42157</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>42192</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>42220</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>42248</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>42283</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>42311</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>42339</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>42402</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>42430</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>42465</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>42493</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>42528</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>42556</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>42584</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>42619</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>42647</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>42675</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>42710</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>42773</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>42801</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>42829</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>42857</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>42892</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>42920</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>42948</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>42983</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>43011</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>43046</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>43074</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>43137</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>43165</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>43193</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>43256</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>43284</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>43319</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>43347</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>43375</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>43410</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>43438</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>43501</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>43529</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>43557</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>43592</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>43620</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>43648</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>43683</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>43711</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>43739</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>43774</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>43802</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>43865</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>43893</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>43984</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>44019</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>44047</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>44110</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>44138</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>44229</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>44257</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>sheet1!$AB$2:$AB$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="160"/>
+                <c:pt idx="0">
+                  <c:v>3.0339190664063551</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.98279372785953</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.98279372785953</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.870386375564173</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.870386375564173</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.870386375564173</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.7172506841640289</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7172506841640289</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.7172506841640289</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.8908194645254852</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.8908194645254852</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.8908194645254852</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.0032379764960311</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.0032379764960311</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.4230655517695818</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.4230655517695818</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.4230655517695818</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.508185338708302</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.508185338708302</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.508185338708302</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.6385109008050018</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.6385109008050018</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.6385109008050018</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.618059674932411</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.618059674932411</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.941908273639712</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.941908273639712</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.941908273639712</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.5437592537540041</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.5437592537540041</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.5437592537540041</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.2486506713817529</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.2486506713817529</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.2486506713817529</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.248717402188817</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.248717402188817</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.4461156611055088</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.4461156611055088</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.4461156611055088</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.6356471804663779</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.6356471804663779</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.6356471804663779</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.7988949086265649</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.7988949086265649</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.7988949086265649</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.7376531923213752</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.7376531923213752</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.7886801378756161</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.7886801378756161</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.7886801378756161</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.8856873553369842</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.8856873553369842</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.8856873553369842</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.9214711268710829</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.9214711268710829</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.9214711268710829</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.6152310888828652</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.6152310888828652</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.5846800125311802</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.5846800125311802</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.5846800125311802</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.6151543533463548</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.6151543533463548</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.6151543533463548</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.6254225435291971</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.6254225435291971</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.6254225435291971</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.5540841167362491</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.5540841167362491</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.4270703099221009</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.4270703099221009</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.4270703099221009</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.3809662491040058</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.3809662491040058</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2.3809662491040058</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2.4522206650398322</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2.4522206650398322</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.4522206650398322</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.398271609255076</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2.398271609255076</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2.599970619256339</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2.599970619256339</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2.599970619256339</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2.7376645962694259</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2.7376645962694259</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2.7376645962694259</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2.5174747290849671</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2.5174747290849671</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2.5174747290849671</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2.67644948447807</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.67644948447807</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2.5541013315103669</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2.5541013315103669</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2.5541013315103669</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2.2848179571313381</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2.2848179571313381</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2.2848179571313381</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2.5744877939507091</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2.5744877939507091</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2.5744877939507091</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2.4725868756926279</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2.4725868756926279</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2.2588853335136179</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2.2588853335136179</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2.2588853335136179</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1.7357464945384891</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.7357464945384891</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.7357464945384891</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1.797489268818623</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1.797489268818623</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1.797489268818623</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1.799874825472529</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1.799874825472529</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1.897563417603692</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1.897563417603692</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1.897563417603692</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1.886195323186129</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1.886195323186129</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1.886195323186129</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1.987054154471664</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1.987054154471664</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1.987054154471664</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1.8508861893484581</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1.8508861893484581</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1.936042945596455</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1.936042945596455</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1.936042945596455</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1.9614454347908039</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>1.9614454347908039</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>1.9614454347908039</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>2.1950851680945651</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>2.1950851680945651</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>2.1950851680945651</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>2.1950851680945651</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>2.1950851680945651</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>2.1950851680945651</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>2.1950851680945651</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>2.1950851680945651</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>2.1950851680945651</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>2.1950851680945651</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>2.1950851680945651</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6224-4DCE-B074-FB9D710B50F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1175235168"/>
+        <c:axId val="1175233504"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>sheet1!$BP$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RPPIYEG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>sheet1!$A$2:$A$161</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="160"/>
+                <c:pt idx="0">
+                  <c:v>38993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39056</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39119</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39147</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39175</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39203</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39238</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39266</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39301</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39329</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39357</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39392</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39420</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39483</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39511</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>39539</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39574</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39602</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39630</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39665</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>39693</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>39728</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>39756</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>39784</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39847</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>39875</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>39910</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>39938</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39966</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40029</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40092</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>40120</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40148</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40211</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>40239</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>40274</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40302</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40330</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>40365</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>40393</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>40428</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>40456</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>40484</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>40519</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>40575</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>40603</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>40638</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>40666</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>40701</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>40729</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>40757</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>40792</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>40820</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>40848</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>40883</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>40946</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>40974</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>41002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>41030</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>41065</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>41093</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>41128</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>41156</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>41184</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>41219</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>41247</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>41310</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>41338</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>41366</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>41401</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>41429</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>41457</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>41492</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>41520</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>41548</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>41583</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>41611</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>41674</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>41702</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>41730</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>41765</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>41793</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>41821</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>41856</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>41884</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>41919</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>41947</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>41975</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>42038</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>42066</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>42101</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>42129</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>42157</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>42192</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>42220</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>42248</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>42283</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>42311</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>42339</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>42402</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>42430</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>42465</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>42493</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>42528</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>42556</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>42584</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>42619</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>42647</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>42675</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>42710</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>42773</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>42801</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>42829</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>42857</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>42892</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>42920</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>42948</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>42983</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>43011</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>43046</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>43074</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>43137</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>43165</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>43193</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>43256</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>43284</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>43319</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>43347</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>43375</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>43410</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>43438</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>43501</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>43529</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>43557</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>43592</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>43620</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>43648</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>43683</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>43711</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>43739</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>43774</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>43802</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>43865</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>43893</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>43984</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>44019</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>44047</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>44110</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>44138</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>44229</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>44257</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>sheet1!$BP$2:$BP$161</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="160"/>
+                <c:pt idx="0">
+                  <c:v>8.7378640776699198E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.7378640776699198E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5714285714285673E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.5714285714285673E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3445491251682408E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3445491251682408E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.3445491251682408E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.2207792207792127E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.2207792207792127E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.2207792207792127E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.11096938775510189</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.11096938775510189</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.11096938775510189</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.13283208020050136</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.13283208020050136</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.12795031055900619</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.12795031055900619</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.12795031055900619</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.0154577883472125E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.0154577883472125E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.0154577883472125E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.0332950631458161E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.0332950631458161E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.0332950631458161E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-3.9823008849557612E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-3.9823008849557612E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-4.6255506607929549E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-4.6255506607929549E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-4.6255506607929549E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.2222222222222539E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.2222222222222539E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.2222222222222539E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.8181818181818177E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.8181818181818177E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.8181818181818177E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.14285714285714293</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.14285714285714293</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.18129330254041576</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.18129330254041576</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.18129330254041576</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.15631929046563187</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.15631929046563187</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.15631929046563187</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9.5744680851063829E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9.5744680851063829E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9.5744680851063829E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.4354838709677331E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.4354838709677331E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.910068426197514E-3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.910068426197514E-3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.910068426197514E-3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-2.2051773729626051E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-2.2051773729626051E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-2.2051773729626051E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-2.7184466019417448E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-2.7184466019417448E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-2.7184466019417448E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-4.0540540540540432E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-4.0540540540540432E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-2.6290165530671886E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-2.6290165530671886E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-2.6290165530671886E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-1.5686274509803866E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-1.5686274509803866E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-1.5686274509803866E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.0181086519114688E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.0181086519114688E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.0999999999999944E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.0999999999999944E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.0999999999999944E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5.2788844621513911E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5.2788844621513911E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5.2788844621513911E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>8.0838323353293356E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>8.0838323353293356E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>8.0838323353293356E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>9.9609374999999889E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>9.9609374999999889E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.10766246362754615</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.10766246362754615</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.10766246362754615</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.10122989593188271</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.10122989593188271</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.10122989593188271</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8.7719298245614044E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.7719298245614044E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8.7719298245614044E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>6.7495559502664379E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>6.7495559502664379E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>6.9176882661996425E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6.9176882661996425E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>6.9176882661996425E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9.7938144329896823E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.7938144329896823E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.7938144329896823E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.10696095076400687</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.10696095076400687</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.10696095076400687</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>8.652246256239593E-2</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>8.652246256239593E-2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>6.7977067977068067E-2</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>6.7977067977068067E-2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>6.7977067977068067E-2</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>4.0688575899843531E-2</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>4.0688575899843531E-2</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>4.0688575899843531E-2</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>3.5276073619631858E-2</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>3.5276073619631858E-2</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>3.5276073619631858E-2</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>7.6569678407350697E-2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>7.6569678407350697E-2</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.10199386503067472</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.10199386503067472</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.10199386503067472</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.10150375939849623</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.10150375939849623</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.10150375939849623</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>8.2962962962962877E-2</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>8.2962962962962877E-2</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>8.2962962962962877E-2</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>4.9786628733997154E-2</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>4.9786628733997154E-2</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>2.0180932498260307E-2</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>2.0180932498260307E-2</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>2.0180932498260307E-2</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>-6.1433447098976496E-3</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-6.1433447098976496E-3</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-6.1433447098976496E-3</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>-1.9151846785225603E-2</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>-1.9151846785225603E-2</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>-1.9151846785225603E-2</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>-5.1490514905149012E-2</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>-5.1490514905149012E-2</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>-7.366984993178706E-2</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>-7.366984993178706E-2</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>-7.366984993178706E-2</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>-7.4175824175824065E-2</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>-7.4175824175824065E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6224-4DCE-B074-FB9D710B50F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>sheet1!$BR$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EHPIYEG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>sheet1!$A$2:$A$161</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="160"/>
+                <c:pt idx="0">
+                  <c:v>38993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39056</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39119</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39147</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39175</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39203</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39238</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39266</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39301</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39329</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39357</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39392</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39420</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39483</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39511</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>39539</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39574</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39602</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39630</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39665</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>39693</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>39728</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>39756</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>39784</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39847</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>39875</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>39910</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>39938</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39966</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40029</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40092</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>40120</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40148</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40211</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>40239</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>40274</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40302</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40330</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>40365</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>40393</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>40428</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>40456</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>40484</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>40519</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>40575</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>40603</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>40638</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>40666</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>40701</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>40729</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>40757</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>40792</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>40820</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>40848</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>40883</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>40946</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>40974</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>41002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>41030</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>41065</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>41093</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>41128</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>41156</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>41184</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>41219</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>41247</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>41310</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>41338</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>41366</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>41401</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>41429</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>41457</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>41492</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>41520</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>41548</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>41583</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>41611</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>41674</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>41702</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>41730</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>41765</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>41793</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>41821</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>41856</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>41884</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>41919</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>41947</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>41975</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>42038</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>42066</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>42101</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>42129</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>42157</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>42192</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>42220</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>42248</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>42283</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>42311</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>42339</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>42402</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>42430</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>42465</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>42493</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>42528</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>42556</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>42584</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>42619</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>42647</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>42675</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>42710</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>42773</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>42801</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>42829</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>42857</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>42892</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>42920</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>42948</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>42983</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>43011</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>43046</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>43074</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>43137</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>43165</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>43193</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>43256</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>43284</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>43319</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>43347</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>43375</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>43410</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>43438</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>43501</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>43529</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>43557</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>43592</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>43620</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>43648</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>43683</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>43711</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>43739</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>43774</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>43802</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>43865</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>43893</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>43928</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>43984</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>44019</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>44047</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>44110</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>44138</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>44229</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>44257</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>sheet1!$BR$2:$BR$161</c:f>
+              <c:numCache>
+                <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
+                <c:ptCount val="160"/>
+                <c:pt idx="0">
+                  <c:v>0.10098176718092571</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10098176718092571</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.7393689986282492E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7393689986282492E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.6205962059620717E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6205962059620717E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.6205962059620717E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.10052219321148829</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.10052219321148829</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.10052219321148829</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.11464968152866242</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.11464968152866242</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.11464968152866242</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.14000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.14000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.13473423980222485</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.13473423980222485</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.13473423980222485</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.9478054567022574E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.9478054567022574E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.9478054567022574E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.3714285714285747E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.3714285714285747E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3714285714285747E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-4.057017543859652E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-4.057017543859652E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-5.4466230936819175E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-5.4466230936819175E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-5.4466230936819175E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-6.593406593406531E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-6.593406593406531E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-6.593406593406531E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.4261555806087972E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.4261555806087972E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.4261555806087972E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.13828571428571423</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.13828571428571423</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.18778801843317969</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.18778801843317969</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.18778801843317969</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.16150442477876098</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.16150442477876098</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.16150442477876098</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9.9576271186440579E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9.9576271186440579E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9.9576271186440579E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.7188755020080353E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.7188755020080353E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9.6993210475275005E-4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>9.6993210475275005E-4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>9.6993210475275005E-4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-2.6666666666666641E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-2.6666666666666641E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-2.6666666666666641E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-3.3718689788053952E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-3.3718689788053952E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-3.3718689788053952E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-4.4103547459252102E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-4.4103547459252102E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-3.391472868217054E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-3.391472868217054E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-3.391472868217054E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-1.8590998043052892E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-1.8590998043052892E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-1.8590998043052892E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-1.9940179461615439E-3</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-1.9940179461615439E-3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-1.9940179461615439E-3</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.6078234704112278E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.6078234704112278E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.4102306920762201E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.4102306920762201E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.4102306920762201E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5.2841475573280131E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5.2841475573280131E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5.2841475573280131E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>8.2917082917083038E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>8.2917082917083038E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>8.2917082917083038E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.10459433040078205</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.10459433040078205</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.10960232783705152</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.10960232783705152</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.10960232783705152</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.10606060606060609</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.10606060606060609</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.10606060606060609</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>9.2250922509225092E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>9.2250922509225092E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>9.2250922509225092E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>6.9911504424778809E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>6.9911504424778809E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>7.5174825174825127E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>7.5174825174825127E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>7.5174825174825127E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.10530821917808217</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.10530821917808217</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.10530821917808217</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.11402027027027027</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.11402027027027027</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.11402027027027027</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>9.263854425144738E-2</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>9.263854425144738E-2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>7.3983739837398324E-2</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>7.3983739837398324E-2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>7.3983739837398324E-2</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>4.6475600309837335E-2</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>4.6475600309837335E-2</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>4.6475600309837335E-2</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>4.094010614101596E-2</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>4.094010614101596E-2</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>4.094010614101596E-2</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>8.8569265707797259E-2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>8.8569265707797259E-2</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.11506434519303571</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.11506434519303571</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.11506434519303571</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.11102886750555145</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.11102886750555145</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.11102886750555145</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>9.3226511289147718E-2</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>9.3226511289147718E-2</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>9.3226511289147718E-2</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>5.5632823365785809E-2</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>5.5632823365785809E-2</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>2.2403258655804364E-2</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>2.2403258655804364E-2</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>2.2403258655804364E-2</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>-2.6648900732845148E-3</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-2.6648900732845148E-3</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-2.6648900732845148E-3</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>-1.9320453031312496E-2</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>-1.9320453031312496E-2</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>-1.9320453031312496E-2</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>-5.5335968379446675E-2</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>-5.5335968379446675E-2</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>-7.7025232403718419E-2</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>-7.7025232403718419E-2</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>-7.7025232403718419E-2</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>-7.7488309953239784E-2</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>-7.7488309953239784E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6224-4DCE-B074-FB9D710B50F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1709338480"/>
+        <c:axId val="1709336400"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="1175235168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1175233504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1175233504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1175235168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1709336400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1709338480"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dateAx>
+        <c:axId val="1709338480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1709336400"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>450272</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>115465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>115453</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>138544</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3EA898D-EF7B-45B0-B2B3-556BD02500B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -832,15 +4617,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BW161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="BY28" sqref="BY28"/>
+      <selection pane="bottomLeft" activeCell="BA6" sqref="BA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.26953125" style="3" customWidth="1"/>
+    <col min="70" max="70" width="8.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:75" ht="71.5" x14ac:dyDescent="0.35">
@@ -33579,7 +37365,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Defined list of variables, and went through different specifications for those
</commit_message>
<xml_diff>
--- a/Complied Data.xlsx
+++ b/Complied Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\R-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258AC2A3-CE24-46A1-B173-1D1DEAF1F438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2B352D-D3E3-439B-93ED-62B8F4B7A3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CG161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="CK141" sqref="CK140:CK141"/>
     </sheetView>
@@ -904,6 +904,7 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.26953125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="14.54296875" customWidth="1"/>
     <col min="22" max="23" width="8.7265625" style="15"/>
     <col min="26" max="27" width="8.7265625" style="15"/>
   </cols>
@@ -37690,8 +37691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B774475B-152D-41DB-8C44-F4758C10BEA0}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>